<commit_message>
add method for obtaining combined data for each category
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="REIT" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Metal" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Commodity" sheetId="6" state="visible" r:id="rId6"/>
@@ -489,17 +489,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IAU</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>iShares Gold Trust</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -507,10 +507,10 @@
         <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>15.17</v>
       </c>
       <c r="G2" t="n">
-        <v>14.52</v>
+        <v>4.26</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -518,12 +518,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DBMF</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>iMGP DBi Managed Futures Strategy ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -533,14 +533,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.85</v>
+        <v>0.14</v>
       </c>
       <c r="F3" t="n">
-        <v>7.81</v>
+        <v>4.57</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -551,28 +551,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MCRO</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IQ Hedge Macro Tracker ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>NasdaqGM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Long-Term Bond</t>
+        </is>
+      </c>
       <c r="E4" t="n">
-        <v>0.67</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>2.5</v>
+        <v>5.35</v>
       </c>
       <c r="G4" t="n">
-        <v>6.59</v>
+        <v>13.98</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -580,32 +584,32 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VIXM</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ProShares VIX Mid-Term Futures ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Trading--Miscellaneous</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.93</v>
+        <v>0.18</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>5.97</v>
       </c>
       <c r="G5" t="n">
-        <v>38.36</v>
+        <v>11.02</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
@@ -616,6 +620,196 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Exchange Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Category Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Dividend Yield</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>5y Std Dev</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Risk Weight</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Asset Weight</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>IAU</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>iShares Gold Trust</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>14.52</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DBMF</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>iMGP DBi Managed Futures Strategy ETF</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Managed Futures</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7.81</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MCRO</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>IQ Hedge Macro Tracker ETF</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>VIXM</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ProShares VIX Mid-Term Futures ETF</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cboe US</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Trading--Miscellaneous</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>38.36</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -902,200 +1096,6 @@
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ticker</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Exchange Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Category Name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Expense Ratio</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Dividend Yield</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>5y Std Dev</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Risk Weight</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Asset Weight</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>FLIA</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Franklin International Aggregate Bond ETF</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Cboe US</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="F2" t="n">
-        <v>15.17</v>
-      </c>
-      <c r="G2" t="n">
-        <v>4.26</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>BILS</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Ultrashort Bond</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="F3" t="n">
-        <v>4.57</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>VCLT</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>NasdaqGM</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Long-Term Bond</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5.35</v>
-      </c>
-      <c r="G4" t="n">
-        <v>13.98</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>VWOB</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>NasdaqGM</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Emerging Markets Bond</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="F5" t="n">
-        <v>5.97</v>
-      </c>
-      <c r="G5" t="n">
-        <v>11.02</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add optimization (MPT) fix asset category
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,13 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="REIT" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Metal" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Commodity" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Currency" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -489,17 +485,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>IAU</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>iShares Gold Trust</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -507,10 +503,10 @@
         <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>15.17</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>4.26</v>
+        <v>14.52</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -518,12 +514,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>DBMF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>iMGP DBi Managed Futures Strategy ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -533,14 +529,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.14</v>
+        <v>0.85</v>
       </c>
       <c r="F3" t="n">
-        <v>4.57</v>
+        <v>7.81</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -551,32 +547,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>MCRO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>IQ Hedge Macro Tracker ETF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Long-Term Bond</t>
-        </is>
-      </c>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="F4" t="n">
-        <v>5.35</v>
+        <v>2.5</v>
       </c>
       <c r="G4" t="n">
-        <v>13.98</v>
+        <v>6.59</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -584,32 +576,32 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>VIXM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>ProShares VIX Mid-Term Futures ETF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Trading--Miscellaneous</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.18</v>
+        <v>0.93</v>
       </c>
       <c r="F5" t="n">
-        <v>5.97</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>11.02</v>
+        <v>38.36</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
@@ -683,17 +675,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IAU</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>iShares Gold Trust</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -701,10 +693,10 @@
         <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>15.17</v>
       </c>
       <c r="G2" t="n">
-        <v>14.52</v>
+        <v>4.26</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -712,12 +704,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DBMF</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>iMGP DBi Managed Futures Strategy ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -727,14 +719,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.85</v>
+        <v>0.14</v>
       </c>
       <c r="F3" t="n">
-        <v>7.81</v>
+        <v>4.57</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -745,28 +737,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MCRO</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IQ Hedge Macro Tracker ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>NasdaqGM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Long-Term Bond</t>
+        </is>
+      </c>
       <c r="E4" t="n">
-        <v>0.67</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>2.5</v>
+        <v>5.35</v>
       </c>
       <c r="G4" t="n">
-        <v>6.59</v>
+        <v>13.98</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -774,32 +770,32 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VIXM</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ProShares VIX Mid-Term Futures ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Trading--Miscellaneous</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.93</v>
+        <v>0.18</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>5.97</v>
       </c>
       <c r="G5" t="n">
-        <v>38.36</v>
+        <v>11.02</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
@@ -1100,108 +1096,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ticker</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ticker</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ticker</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ticker</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add monte carlo VaR calculation add VaR conversion to USD
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -485,17 +485,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IAU</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>iShares Gold Trust</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -503,10 +503,10 @@
         <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>15.17</v>
       </c>
       <c r="G2" t="n">
-        <v>14.52</v>
+        <v>4.26</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -514,12 +514,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DBMF</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>iMGP DBi Managed Futures Strategy ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -529,14 +529,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.85</v>
+        <v>0.14</v>
       </c>
       <c r="F3" t="n">
-        <v>7.81</v>
+        <v>4.57</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -547,28 +547,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MCRO</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IQ Hedge Macro Tracker ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>NasdaqGM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Long-Term Bond</t>
+        </is>
+      </c>
       <c r="E4" t="n">
-        <v>0.67</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>2.5</v>
+        <v>5.35</v>
       </c>
       <c r="G4" t="n">
-        <v>6.59</v>
+        <v>13.98</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -576,32 +580,32 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VIXM</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ProShares VIX Mid-Term Futures ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Trading--Miscellaneous</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.93</v>
+        <v>0.18</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>5.97</v>
       </c>
       <c r="G5" t="n">
-        <v>38.36</v>
+        <v>11.02</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
@@ -612,6 +616,299 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Exchange Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Category Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Dividend Yield</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>5y Std Dev</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Risk Weight</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Asset Weight</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Vanguard 500 Index Fund</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="G2" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FLCA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Franklin FTSE Canada ETF</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="G3" t="n">
+        <v>20.54</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1329.T</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>iShares Core Nikkei 225 ETF</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tokyo</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="G4" t="n">
+        <v>16.89</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FLAU</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Franklin FTSE Australia ETF</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="G5" t="n">
+        <v>23.72</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="G6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -675,17 +972,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>IAU</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>iShares Gold Trust</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -693,10 +990,10 @@
         <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>15.17</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>4.26</v>
+        <v>14.52</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -704,12 +1001,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>DBMF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>iMGP DBi Managed Futures Strategy ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -719,14 +1016,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.14</v>
+        <v>0.85</v>
       </c>
       <c r="F3" t="n">
-        <v>4.57</v>
+        <v>7.81</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -737,32 +1034,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>MCRO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>IQ Hedge Macro Tracker ETF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Long-Term Bond</t>
-        </is>
-      </c>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="F4" t="n">
-        <v>5.35</v>
+        <v>2.5</v>
       </c>
       <c r="G4" t="n">
-        <v>13.98</v>
+        <v>6.59</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -770,328 +1063,35 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>VIXM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>ProShares VIX Mid-Term Futures ETF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Trading--Miscellaneous</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.18</v>
+        <v>0.93</v>
       </c>
       <c r="F5" t="n">
-        <v>5.97</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>11.02</v>
+        <v>38.36</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ticker</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Exchange Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Category Name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Expense Ratio</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Dividend Yield</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>5y Std Dev</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Risk Weight</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Asset Weight</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>VOO</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Vanguard 500 Index Fund</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.62</v>
-      </c>
-      <c r="G2" t="n">
-        <v>18.7</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>FLCA</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Franklin FTSE Canada ETF</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3.17</v>
-      </c>
-      <c r="G3" t="n">
-        <v>20.54</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1329.T</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>iShares Core Nikkei 225 ETF</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Tokyo</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1.82</v>
-      </c>
-      <c r="G4" t="n">
-        <v>16.89</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>FLAU</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Franklin FTSE Australia ETF</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="F5" t="n">
-        <v>4.72</v>
-      </c>
-      <c r="G5" t="n">
-        <v>23.72</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="G6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="G7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="G8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add monte carlo VaR calculation for each category exclude foreign ETF from the ETF.xlsx
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,28 +485,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>Vanguard 500 Index Fund</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
+      </c>
       <c r="E2" t="n">
-        <v>0.25</v>
+        <v>0.14</v>
       </c>
       <c r="F2" t="n">
-        <v>15.17</v>
+        <v>1.62</v>
       </c>
       <c r="G2" t="n">
-        <v>4.26</v>
+        <v>18.7</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -514,12 +518,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>FLCA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>Franklin FTSE Canada ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -529,17 +533,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.14</v>
+        <v>0.09</v>
       </c>
       <c r="F3" t="n">
-        <v>4.57</v>
+        <v>3.17</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -547,32 +551,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>FLJP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Long-Term Bond</t>
+          <t>Japan Stock</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="F4" t="n">
-        <v>5.35</v>
+        <v>2.24</v>
       </c>
       <c r="G4" t="n">
-        <v>13.98</v>
+        <v>15.34</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -580,35 +584,134 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="F5" t="n">
-        <v>5.97</v>
+        <v>4.72</v>
       </c>
       <c r="G5" t="n">
-        <v>11.02</v>
+        <v>23.72</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="G6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -621,7 +724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,32 +782,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vanguard 500 Index Fund</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
+          <t>Cboe US</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.14</v>
+        <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>1.62</v>
+        <v>15.17</v>
       </c>
       <c r="G2" t="n">
-        <v>18.7</v>
+        <v>4.26</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -712,12 +811,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FLCA</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Franklin FTSE Canada ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -727,17 +826,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.09</v>
+        <v>0.14</v>
       </c>
       <c r="F3" t="n">
-        <v>3.17</v>
+        <v>4.57</v>
       </c>
       <c r="G3" t="n">
-        <v>20.54</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -745,28 +844,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1329.T</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>iShares Core Nikkei 225 ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Tokyo</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>NasdaqGM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Long-Term Bond</t>
+        </is>
+      </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>1.82</v>
+        <v>5.35</v>
       </c>
       <c r="G4" t="n">
-        <v>16.89</v>
+        <v>13.98</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -774,134 +877,35 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="F5" t="n">
-        <v>4.72</v>
+        <v>5.97</v>
       </c>
       <c r="G5" t="n">
-        <v>23.72</v>
+        <v>11.02</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="G6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="G7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="G8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add PMPT optimization with monte carlo simulation add Risk Free Rate from 3 month T-Bill
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,32 +485,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vanguard 500 Index Fund</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
+          <t>Cboe US</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.14</v>
+        <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>1.62</v>
+        <v>15.17</v>
       </c>
       <c r="G2" t="n">
-        <v>18.7</v>
+        <v>4.26</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -518,12 +514,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FLCA</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Franklin FTSE Canada ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -533,17 +529,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.09</v>
+        <v>0.14</v>
       </c>
       <c r="F3" t="n">
-        <v>3.17</v>
+        <v>4.57</v>
       </c>
       <c r="G3" t="n">
-        <v>20.54</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -551,32 +547,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLJP</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Franklin FTSE Japan ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Japan Stock</t>
+          <t>Long-Term Bond</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>2.24</v>
+        <v>5.35</v>
       </c>
       <c r="G4" t="n">
-        <v>15.34</v>
+        <v>13.98</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -584,134 +580,35 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="F5" t="n">
-        <v>4.72</v>
+        <v>5.97</v>
       </c>
       <c r="G5" t="n">
-        <v>23.72</v>
+        <v>11.02</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="G6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="G7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="G8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -724,7 +621,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,28 +679,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>Vanguard 500 Index Fund</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
+      </c>
       <c r="E2" t="n">
-        <v>0.25</v>
+        <v>0.14</v>
       </c>
       <c r="F2" t="n">
-        <v>15.17</v>
+        <v>1.62</v>
       </c>
       <c r="G2" t="n">
-        <v>4.26</v>
+        <v>18.7</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -811,12 +712,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>FLCA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>Franklin FTSE Canada ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -826,17 +727,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.14</v>
+        <v>0.09</v>
       </c>
       <c r="F3" t="n">
-        <v>4.57</v>
+        <v>3.17</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -844,32 +745,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>FLJP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Long-Term Bond</t>
+          <t>Japan Stock</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="F4" t="n">
-        <v>5.35</v>
+        <v>2.24</v>
       </c>
       <c r="G4" t="n">
-        <v>13.98</v>
+        <v>15.34</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -877,35 +778,134 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="F5" t="n">
-        <v>5.97</v>
+        <v>4.72</v>
       </c>
       <c r="G5" t="n">
-        <v>11.02</v>
+        <v>23.72</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="G6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add yearly and monthly downside risk for each asset category add plot asset category chart
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,28 +485,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>Vanguard 500 Index Fund</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
+      </c>
       <c r="E2" t="n">
-        <v>0.25</v>
+        <v>0.14</v>
       </c>
       <c r="F2" t="n">
-        <v>15.17</v>
+        <v>1.62</v>
       </c>
       <c r="G2" t="n">
-        <v>4.26</v>
+        <v>18.7</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -514,12 +518,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>FLCA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>Franklin FTSE Canada ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -529,17 +533,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.14</v>
+        <v>0.09</v>
       </c>
       <c r="F3" t="n">
-        <v>4.57</v>
+        <v>3.17</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -547,32 +551,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>FLJP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Long-Term Bond</t>
+          <t>Japan Stock</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="F4" t="n">
-        <v>5.35</v>
+        <v>2.24</v>
       </c>
       <c r="G4" t="n">
-        <v>13.98</v>
+        <v>15.34</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -580,35 +584,134 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="F5" t="n">
-        <v>5.97</v>
+        <v>4.72</v>
       </c>
       <c r="G5" t="n">
-        <v>11.02</v>
+        <v>23.72</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="G6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -621,7 +724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,32 +782,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vanguard 500 Index Fund</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
+          <t>Cboe US</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.14</v>
+        <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>1.62</v>
+        <v>15.17</v>
       </c>
       <c r="G2" t="n">
-        <v>18.7</v>
+        <v>4.26</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -712,12 +811,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FLCA</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Franklin FTSE Canada ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -727,17 +826,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.09</v>
+        <v>0.14</v>
       </c>
       <c r="F3" t="n">
-        <v>3.17</v>
+        <v>4.57</v>
       </c>
       <c r="G3" t="n">
-        <v>20.54</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -745,32 +844,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLJP</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Franklin FTSE Japan ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Japan Stock</t>
+          <t>Long-Term Bond</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>2.24</v>
+        <v>5.35</v>
       </c>
       <c r="G4" t="n">
-        <v>15.34</v>
+        <v>13.98</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -778,134 +877,35 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
       <c r="F5" t="n">
-        <v>4.72</v>
+        <v>5.97</v>
       </c>
       <c r="G5" t="n">
-        <v>23.72</v>
+        <v>11.02</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="G6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="G7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="G8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix sortino ratio optimizer fix sharp ratio optimizer fix category avg historical data
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,32 +485,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vanguard 500 Index Fund</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
+          <t>Cboe US</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.14</v>
+        <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>1.62</v>
+        <v>15.17</v>
       </c>
       <c r="G2" t="n">
-        <v>18.7</v>
+        <v>4.26</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -518,12 +514,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FLCA</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Franklin FTSE Canada ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -533,17 +529,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.09</v>
+        <v>0.14</v>
       </c>
       <c r="F3" t="n">
-        <v>3.17</v>
+        <v>4.57</v>
       </c>
       <c r="G3" t="n">
-        <v>20.54</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -551,32 +547,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLJP</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Franklin FTSE Japan ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Japan Stock</t>
+          <t>Long-Term Bond</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>2.24</v>
+        <v>5.35</v>
       </c>
       <c r="G4" t="n">
-        <v>15.34</v>
+        <v>13.98</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -584,134 +580,35 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
       <c r="F5" t="n">
-        <v>4.72</v>
+        <v>5.97</v>
       </c>
       <c r="G5" t="n">
-        <v>23.72</v>
+        <v>11.02</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="G6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="G7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="G8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -782,17 +679,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>IAU</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>iShares Gold Trust</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -800,10 +697,10 @@
         <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>15.17</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>4.26</v>
+        <v>14.52</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -811,12 +708,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>DBMF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>iMGP DBi Managed Futures Strategy ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -826,14 +723,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.14</v>
+        <v>0.85</v>
       </c>
       <c r="F3" t="n">
-        <v>4.57</v>
+        <v>7.81</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -844,32 +741,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>MCRO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>IQ Hedge Macro Tracker ETF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Long-Term Bond</t>
-        </is>
-      </c>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="F4" t="n">
-        <v>5.35</v>
+        <v>2.5</v>
       </c>
       <c r="G4" t="n">
-        <v>13.98</v>
+        <v>6.59</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -877,32 +770,32 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>VIXM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>ProShares VIX Mid-Term Futures ETF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Trading--Miscellaneous</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.2</v>
+        <v>0.93</v>
       </c>
       <c r="F5" t="n">
-        <v>5.97</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>11.02</v>
+        <v>38.36</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
@@ -918,7 +811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -976,12 +869,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IAU</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>iShares Gold Trust</t>
+          <t>Vanguard 500 Index Fund</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -989,15 +882,19 @@
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
+      </c>
       <c r="E2" t="n">
-        <v>0.25</v>
+        <v>0.14</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1.62</v>
       </c>
       <c r="G2" t="n">
-        <v>14.52</v>
+        <v>18.7</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -1005,12 +902,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DBMF</t>
+          <t>FLCA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>iMGP DBi Managed Futures Strategy ETF</t>
+          <t>Franklin FTSE Canada ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1020,17 +917,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.85</v>
+        <v>0.09</v>
       </c>
       <c r="F3" t="n">
-        <v>7.81</v>
+        <v>3.17</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -1038,12 +935,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MCRO</t>
+          <t>FLJP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IQ Hedge Macro Tracker ETF</t>
+          <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1051,15 +948,19 @@
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Japan Stock</t>
+        </is>
+      </c>
       <c r="E4" t="n">
-        <v>0.67</v>
+        <v>0.09</v>
       </c>
       <c r="F4" t="n">
-        <v>2.5</v>
+        <v>2.24</v>
       </c>
       <c r="G4" t="n">
-        <v>6.59</v>
+        <v>15.34</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -1067,35 +968,134 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VIXM</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ProShares VIX Mid-Term Futures ETF</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Trading--Miscellaneous</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.93</v>
+        <v>0.09</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>4.72</v>
       </c>
       <c r="G5" t="n">
-        <v>38.36</v>
+        <v>23.72</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="G6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix fetch historical data resampled to daily
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,28 +485,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>Vanguard 500 Index Fund</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
+      </c>
       <c r="E2" t="n">
-        <v>0.25</v>
+        <v>0.14</v>
       </c>
       <c r="F2" t="n">
-        <v>15.17</v>
+        <v>1.62</v>
       </c>
       <c r="G2" t="n">
-        <v>4.26</v>
+        <v>18.7</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -514,12 +518,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>FLCA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>Franklin FTSE Canada ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -529,17 +533,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.14</v>
+        <v>0.09</v>
       </c>
       <c r="F3" t="n">
-        <v>4.57</v>
+        <v>3.17</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -547,32 +551,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>FLJP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Long-Term Bond</t>
+          <t>Japan Stock</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="F4" t="n">
-        <v>5.35</v>
+        <v>2.24</v>
       </c>
       <c r="G4" t="n">
-        <v>13.98</v>
+        <v>15.34</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -580,35 +584,134 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.2</v>
+        <v>0.09</v>
       </c>
       <c r="F5" t="n">
-        <v>5.97</v>
+        <v>4.72</v>
       </c>
       <c r="G5" t="n">
-        <v>11.02</v>
+        <v>23.72</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="G6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -811,7 +914,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -869,32 +972,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vanguard 500 Index Fund</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
+          <t>Cboe US</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.14</v>
+        <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>1.62</v>
+        <v>15.17</v>
       </c>
       <c r="G2" t="n">
-        <v>18.7</v>
+        <v>4.26</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -902,12 +1001,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FLCA</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Franklin FTSE Canada ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -917,17 +1016,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.09</v>
+        <v>0.14</v>
       </c>
       <c r="F3" t="n">
-        <v>3.17</v>
+        <v>4.57</v>
       </c>
       <c r="G3" t="n">
-        <v>20.54</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -935,32 +1034,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLJP</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Franklin FTSE Japan ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Japan Stock</t>
+          <t>Long-Term Bond</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>2.24</v>
+        <v>5.35</v>
       </c>
       <c r="G4" t="n">
-        <v>15.34</v>
+        <v>13.98</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -968,134 +1067,35 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
       <c r="F5" t="n">
-        <v>4.72</v>
+        <v>5.97</v>
       </c>
       <c r="G5" t="n">
-        <v>23.72</v>
+        <v>11.02</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="G6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="G7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="G8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add Sub Category as a variable
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,40 +443,45 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Sub Category</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Exchange Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Category Name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Expense Ratio</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>5y Std Dev</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Risk Weight</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Asset Weight</t>
         </is>
@@ -485,233 +490,150 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vanguard 500 Index Fund</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0.14</v>
-      </c>
+          <t>Cboe US</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>1.62</v>
+        <v>0.25</v>
       </c>
       <c r="G2" t="n">
-        <v>18.7</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
+        <v>15.17</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4.26</v>
+      </c>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FLCA</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Franklin FTSE Canada ETF</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0.09</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Ultrashort Bond</t>
+        </is>
       </c>
       <c r="F3" t="n">
-        <v>3.17</v>
+        <v>0.14</v>
       </c>
       <c r="G3" t="n">
-        <v>20.54</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
+        <v>4.57</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLJP</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Franklin FTSE Japan ETF</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Japan Stock</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0.09</v>
+          <t>NasdaqGM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Long-Term Bond</t>
+        </is>
       </c>
       <c r="F4" t="n">
-        <v>2.24</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>15.34</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
+        <v>5.35</v>
+      </c>
+      <c r="H4" t="n">
+        <v>13.98</v>
+      </c>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0.09</v>
+          <t>NasdaqGM</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Emerging Markets Bond</t>
+        </is>
       </c>
       <c r="F5" t="n">
-        <v>4.72</v>
+        <v>0.2</v>
       </c>
       <c r="G5" t="n">
-        <v>23.72</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
+        <v>5.97</v>
+      </c>
+      <c r="H5" t="n">
+        <v>11.02</v>
+      </c>
       <c r="I5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="G6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="G7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="G8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -724,7 +646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -740,40 +662,45 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Sub Category</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Exchange Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Category Name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Expense Ratio</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>5y Std Dev</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Risk Weight</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Asset Weight</t>
         </is>
@@ -787,26 +714,31 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Gold</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>iShares Gold Trust</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="n">
         <v>0.25</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>14.52</v>
       </c>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -816,30 +748,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Managed Futures</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>iMGP DBi Managed Futures Strategy ETF</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Managed Futures</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.85</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>7.81</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -849,26 +786,31 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Global Macro</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>IQ Hedge Macro Tracker ETF</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
         <v>0.67</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>2.5</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>6.59</v>
       </c>
-      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -878,30 +820,35 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>VIX Futures</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>ProShares VIX Mid-Term Futures ETF</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Cboe US</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Trading--Miscellaneous</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.93</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>0</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>38.36</v>
       </c>
-      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -914,7 +861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -930,40 +877,45 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Sub Category</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Exchange Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Category Name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Expense Ratio</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>5y Std Dev</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Risk Weight</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Asset Weight</t>
         </is>
@@ -972,130 +924,268 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>0.25</v>
+          <t>Vanguard 500 Index Fund</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
       </c>
       <c r="F2" t="n">
-        <v>15.17</v>
+        <v>0.14</v>
       </c>
       <c r="G2" t="n">
-        <v>4.26</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
+        <v>1.62</v>
+      </c>
+      <c r="H2" t="n">
+        <v>18.7</v>
+      </c>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>FLCA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Franklin FTSE Canada ETF</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Ultrashort Bond</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0.14</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
       </c>
       <c r="F3" t="n">
-        <v>4.57</v>
+        <v>0.09</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
+        <v>3.17</v>
+      </c>
+      <c r="H3" t="n">
+        <v>20.54</v>
+      </c>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>FLJP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Long-Term Bond</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0.07000000000000001</v>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Japan Stock</t>
+        </is>
       </c>
       <c r="F4" t="n">
-        <v>5.35</v>
+        <v>0.09</v>
       </c>
       <c r="G4" t="n">
-        <v>13.98</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
+        <v>2.24</v>
+      </c>
+      <c r="H4" t="n">
+        <v>15.34</v>
+      </c>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0.2</v>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
       </c>
       <c r="F5" t="n">
-        <v>5.97</v>
+        <v>0.09</v>
       </c>
       <c r="G5" t="n">
-        <v>11.02</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
+        <v>4.72</v>
+      </c>
+      <c r="H5" t="n">
+        <v>23.72</v>
+      </c>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Traditional</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="H6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Traditional</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="H7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Traditional</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="H8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix bulk update securities
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,7 +490,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -500,23 +500,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>Vanguard 500 Index Fund</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
+      </c>
       <c r="F2" t="n">
-        <v>0.25</v>
+        <v>0.14</v>
       </c>
       <c r="G2" t="n">
-        <v>15.17</v>
+        <v>1.62</v>
       </c>
       <c r="H2" t="n">
-        <v>4.26</v>
+        <v>18.7</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -524,7 +528,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>FLCA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -534,7 +538,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>Franklin FTSE Canada ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -544,17 +548,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.14</v>
+        <v>0.09</v>
       </c>
       <c r="G3" t="n">
-        <v>4.57</v>
+        <v>3.17</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -562,7 +566,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>FLJP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -572,27 +576,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Long-Term Bond</t>
+          <t>Japan Stock</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="G4" t="n">
-        <v>5.35</v>
+        <v>2.24</v>
       </c>
       <c r="H4" t="n">
-        <v>13.98</v>
+        <v>15.34</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -600,7 +604,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -610,30 +614,144 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.2</v>
+        <v>0.09</v>
       </c>
       <c r="G5" t="n">
-        <v>5.97</v>
+        <v>4.72</v>
       </c>
       <c r="H5" t="n">
-        <v>11.02</v>
+        <v>23.72</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Traditional</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="H6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Traditional</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="H7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Traditional</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="H8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -709,22 +827,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IAU</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Gold</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>iShares Gold Trust</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -732,10 +850,10 @@
         <v>0.25</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>15.17</v>
       </c>
       <c r="H2" t="n">
-        <v>14.52</v>
+        <v>4.26</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -743,17 +861,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DBMF</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>iMGP DBi Managed Futures Strategy ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -763,14 +881,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.85</v>
+        <v>0.14</v>
       </c>
       <c r="G3" t="n">
-        <v>7.81</v>
+        <v>4.57</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -781,33 +899,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MCRO</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Global Macro</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IQ Hedge Macro Tracker ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>NasdaqGM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Long-Term Bond</t>
+        </is>
+      </c>
       <c r="F4" t="n">
-        <v>0.67</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>2.5</v>
+        <v>5.35</v>
       </c>
       <c r="H4" t="n">
-        <v>6.59</v>
+        <v>13.98</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -815,37 +937,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VIXM</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VIX Futures</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ProShares VIX Mid-Term Futures ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Trading--Miscellaneous</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.93</v>
+        <v>0.2</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>5.97</v>
       </c>
       <c r="H5" t="n">
-        <v>38.36</v>
+        <v>11.02</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -861,7 +983,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -924,17 +1046,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>IAU</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Gold</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vanguard 500 Index Fund</t>
+          <t>iShares Gold Trust</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -942,19 +1064,15 @@
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>0.14</v>
+        <v>0.25</v>
       </c>
       <c r="G2" t="n">
-        <v>1.62</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>18.7</v>
+        <v>14.52</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -962,17 +1080,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FLCA</t>
+          <t>DBMF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Franklin FTSE Canada ETF</t>
+          <t>iMGP DBi Managed Futures Strategy ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -982,17 +1100,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.09</v>
+        <v>0.85</v>
       </c>
       <c r="G3" t="n">
-        <v>3.17</v>
+        <v>7.81</v>
       </c>
       <c r="H3" t="n">
-        <v>20.54</v>
+        <v>0</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -1000,17 +1118,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLJP</t>
+          <t>MCRO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Global Macro</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Franklin FTSE Japan ETF</t>
+          <t>IQ Hedge Macro Tracker ETF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1018,19 +1136,15 @@
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Japan Stock</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.09</v>
+        <v>0.67</v>
       </c>
       <c r="G4" t="n">
-        <v>2.24</v>
+        <v>2.5</v>
       </c>
       <c r="H4" t="n">
-        <v>15.34</v>
+        <v>6.59</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -1038,154 +1152,40 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>VIXM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>VIX Futures</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>ProShares VIX Mid-Term Futures ETF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Trading--Miscellaneous</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.09</v>
+        <v>0.93</v>
       </c>
       <c r="G5" t="n">
-        <v>4.72</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>23.72</v>
+        <v>38.36</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Traditional</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="G6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="H6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Traditional</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="G7" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="H7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Traditional</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="G8" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="H8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add PyPortfolioOpt optimizer add grouped_securities a dictionary by category and sub-category
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -827,22 +827,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>IAU</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Gold</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>iShares Gold Trust</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -850,10 +850,10 @@
         <v>0.25</v>
       </c>
       <c r="G2" t="n">
-        <v>15.17</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>4.26</v>
+        <v>14.52</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -861,17 +861,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>DBMF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>iMGP DBi Managed Futures Strategy ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -881,14 +881,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.14</v>
+        <v>0.85</v>
       </c>
       <c r="G3" t="n">
-        <v>4.57</v>
+        <v>7.81</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -899,37 +899,33 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>MCRO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Global Macro</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>IQ Hedge Macro Tracker ETF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Long-Term Bond</t>
-        </is>
-      </c>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="G4" t="n">
-        <v>5.35</v>
+        <v>2.5</v>
       </c>
       <c r="H4" t="n">
-        <v>13.98</v>
+        <v>6.59</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -937,37 +933,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>VIXM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>VIX Futures</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>ProShares VIX Mid-Term Futures ETF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Trading--Miscellaneous</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.2</v>
+        <v>0.93</v>
       </c>
       <c r="G5" t="n">
-        <v>5.97</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>11.02</v>
+        <v>38.36</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -1046,22 +1042,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IAU</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Gold</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>iShares Gold Trust</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1069,10 +1065,10 @@
         <v>0.25</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>15.17</v>
       </c>
       <c r="H2" t="n">
-        <v>14.52</v>
+        <v>4.26</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -1080,17 +1076,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DBMF</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>iMGP DBi Managed Futures Strategy ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1100,14 +1096,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.85</v>
+        <v>0.14</v>
       </c>
       <c r="G3" t="n">
-        <v>7.81</v>
+        <v>4.57</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -1118,33 +1114,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MCRO</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Global Macro</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IQ Hedge Macro Tracker ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>NasdaqGM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Long-Term Bond</t>
+        </is>
+      </c>
       <c r="F4" t="n">
-        <v>0.67</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>2.5</v>
+        <v>5.35</v>
       </c>
       <c r="H4" t="n">
-        <v>6.59</v>
+        <v>13.98</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -1152,37 +1152,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VIXM</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VIX Futures</t>
+          <t>Traditional</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ProShares VIX Mid-Term Futures ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Trading--Miscellaneous</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.93</v>
+        <v>0.2</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>5.97</v>
       </c>
       <c r="H5" t="n">
-        <v>38.36</v>
+        <v>11.02</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>

</xml_diff>

<commit_message>
add aggregated_data_calculator calculates average adjusted returns and average historical data
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,7 +490,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -500,27 +500,23 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vanguard 500 Index Fund</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
+          <t>Cboe US</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>0.14</v>
+        <v>0.0025</v>
       </c>
       <c r="G2" t="n">
-        <v>1.62</v>
+        <v>0.1517</v>
       </c>
       <c r="H2" t="n">
-        <v>18.7</v>
+        <v>4.26</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -528,7 +524,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FLCA</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -538,7 +534,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Franklin FTSE Canada ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -548,17 +544,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.09</v>
+        <v>0.00135</v>
       </c>
       <c r="G3" t="n">
-        <v>3.17</v>
+        <v>0.0457</v>
       </c>
       <c r="H3" t="n">
-        <v>20.54</v>
+        <v>0</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -566,7 +562,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLJP</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -576,27 +572,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Franklin FTSE Japan ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Japan Stock</t>
+          <t>Long-Term Bond</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.09</v>
+        <v>0.0007</v>
       </c>
       <c r="G4" t="n">
-        <v>2.24</v>
+        <v>0.0535</v>
       </c>
       <c r="H4" t="n">
-        <v>15.34</v>
+        <v>13.98</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -604,7 +600,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -614,144 +610,30 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.09</v>
+        <v>0.002</v>
       </c>
       <c r="G5" t="n">
-        <v>4.72</v>
+        <v>0.0597</v>
       </c>
       <c r="H5" t="n">
-        <v>23.72</v>
+        <v>11.02</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Traditional</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="G6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="H6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Traditional</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="G7" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="H7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Traditional</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="G8" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="H8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -847,7 +729,7 @@
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>0.25</v>
+        <v>0.0025</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -885,10 +767,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.85</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>7.81</v>
+        <v>0.0781</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -919,10 +801,10 @@
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.67</v>
+        <v>0.0067</v>
       </c>
       <c r="G4" t="n">
-        <v>2.5</v>
+        <v>0.025</v>
       </c>
       <c r="H4" t="n">
         <v>6.59</v>
@@ -957,7 +839,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.93</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -979,7 +861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1042,7 +924,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1052,23 +934,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>Vanguard 500 Index Fund</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
+      </c>
       <c r="F2" t="n">
-        <v>0.25</v>
+        <v>0.0014</v>
       </c>
       <c r="G2" t="n">
-        <v>15.17</v>
+        <v>0.0162</v>
       </c>
       <c r="H2" t="n">
-        <v>4.26</v>
+        <v>18.7</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -1076,7 +962,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>FLCA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1086,7 +972,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>Franklin FTSE Canada ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1096,17 +982,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.14</v>
+        <v>0.0009</v>
       </c>
       <c r="G3" t="n">
-        <v>4.57</v>
+        <v>0.0317</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -1114,7 +1000,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>FLJP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1124,27 +1010,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Long-Term Bond</t>
+          <t>Japan Stock</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.0009</v>
       </c>
       <c r="G4" t="n">
-        <v>5.35</v>
+        <v>0.0224</v>
       </c>
       <c r="H4" t="n">
-        <v>13.98</v>
+        <v>15.34</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -1152,7 +1038,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1162,30 +1048,144 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.2</v>
+        <v>0.0009</v>
       </c>
       <c r="G5" t="n">
-        <v>5.97</v>
+        <v>0.0472</v>
       </c>
       <c r="H5" t="n">
-        <v>11.02</v>
+        <v>23.72</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Traditional</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0375</v>
+      </c>
+      <c r="H6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Traditional</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0007</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="H7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Traditional</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0007</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0339</v>
+      </c>
+      <c r="H8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix pypfopt_optimizer.py return portfolio metrics add category_security.py add category_security_manager.py
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,33 +490,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Traditional Equity</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>Vanguard 500 Index Fund</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
+      </c>
       <c r="F2" t="n">
-        <v>0.0025</v>
+        <v>0.0004</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1517</v>
+        <v>0.0162</v>
       </c>
       <c r="H2" t="n">
-        <v>4.26</v>
+        <v>18.7</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -524,17 +528,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>FLCA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Traditional Equity</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>Franklin FTSE Canada ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -544,17 +548,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.00135</v>
+        <v>0.0009</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0457</v>
+        <v>0.0317</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -562,37 +566,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>FLJP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Traditional Equity</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Long-Term Bond</t>
+          <t>Japan Stock</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.0007</v>
+        <v>0.0009</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0535</v>
+        <v>0.0224</v>
       </c>
       <c r="H4" t="n">
-        <v>13.98</v>
+        <v>15.34</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -600,40 +604,154 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Traditional Equity</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.002</v>
+        <v>0.0009</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0597</v>
+        <v>0.0472</v>
       </c>
       <c r="H5" t="n">
-        <v>11.02</v>
+        <v>23.72</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Traditional Equity</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0375</v>
+      </c>
+      <c r="H6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Traditional Equity</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0007</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="H7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Traditional Equity</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0007</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0339</v>
+      </c>
+      <c r="H8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -709,22 +827,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IAU</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Gold</t>
+          <t>Traditional Bond</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>iShares Gold Trust</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -732,10 +850,10 @@
         <v>0.0025</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.1517</v>
       </c>
       <c r="H2" t="n">
-        <v>14.52</v>
+        <v>4.26</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -743,17 +861,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DBMF</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Traditional Bond</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>iMGP DBi Managed Futures Strategy ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -763,14 +881,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.00135</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0781</v>
+        <v>0.0457</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -781,33 +899,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MCRO</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Global Macro</t>
+          <t>Traditional Bond</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IQ Hedge Macro Tracker ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>NasdaqGM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Long-Term Bond</t>
+        </is>
+      </c>
       <c r="F4" t="n">
-        <v>0.0067</v>
+        <v>0.0007</v>
       </c>
       <c r="G4" t="n">
-        <v>0.025</v>
+        <v>0.0535</v>
       </c>
       <c r="H4" t="n">
-        <v>6.59</v>
+        <v>13.98</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -815,37 +937,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VIXM</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VIX Futures</t>
+          <t>Traditional Bond</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ProShares VIX Mid-Term Futures ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Trading--Miscellaneous</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.009299999999999999</v>
+        <v>0.002</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.0597</v>
       </c>
       <c r="H5" t="n">
-        <v>38.36</v>
+        <v>11.02</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -861,7 +983,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -924,17 +1046,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>IAU</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Metal</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vanguard 500 Index Fund</t>
+          <t>iShares Gold Trust</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -942,19 +1064,15 @@
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>0.0014</v>
+        <v>0.0025</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0162</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>18.7</v>
+        <v>14.52</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -962,17 +1080,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FLCA</t>
+          <t>DBMF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Franklin FTSE Canada ETF</t>
+          <t>iMGP DBi Managed Futures Strategy ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -982,17 +1100,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.0009</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0317</v>
+        <v>0.0781</v>
       </c>
       <c r="H3" t="n">
-        <v>20.54</v>
+        <v>0</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -1000,17 +1118,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLJP</t>
+          <t>MCRO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>Global Macro</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Franklin FTSE Japan ETF</t>
+          <t>IQ Hedge Macro Tracker ETF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1018,19 +1136,15 @@
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Japan Stock</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.0009</v>
+        <v>0.0067</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0224</v>
+        <v>0.025</v>
       </c>
       <c r="H4" t="n">
-        <v>15.34</v>
+        <v>6.59</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -1038,154 +1152,40 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>VIXM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Traditional</t>
+          <t>VIX Futures</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>ProShares VIX Mid-Term Futures ETF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Trading--Miscellaneous</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.0009</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0472</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>23.72</v>
+        <v>38.36</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Traditional</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>0.0009</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.0375</v>
-      </c>
-      <c r="H6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Traditional</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.0333</v>
-      </c>
-      <c r="H7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Traditional</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.0339</v>
-      </c>
-      <c r="H8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix pypfopt_optimizer.py constraint format add category_security.py change aggregated_data_calculator.py conversion frequency to Month add category_security_manager.py group_aggregated_data
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bond" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alternative" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Equity" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,37 +490,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>FLIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Traditional Equity</t>
+          <t>Traditional Bond</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vanguard 500 Index Fund</t>
+          <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Large Blend</t>
-        </is>
-      </c>
+          <t>Cboe US</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>0.0004</v>
+        <v>0.0025</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0162</v>
+        <v>0.1517</v>
       </c>
       <c r="H2" t="n">
-        <v>18.7</v>
+        <v>4.26</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -528,17 +524,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FLCA</t>
+          <t>BILS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Traditional Equity</t>
+          <t>Traditional Bond</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Franklin FTSE Canada ETF</t>
+          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -548,17 +544,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Ultrashort Bond</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.0009</v>
+        <v>0.00135</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0317</v>
+        <v>0.0457</v>
       </c>
       <c r="H3" t="n">
-        <v>20.54</v>
+        <v>0</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -566,37 +562,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLJP</t>
+          <t>VCLT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Traditional Equity</t>
+          <t>Traditional Bond</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Franklin FTSE Japan ETF</t>
+          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Japan Stock</t>
+          <t>Long-Term Bond</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.0009</v>
+        <v>0.0007</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0224</v>
+        <v>0.0535</v>
       </c>
       <c r="H4" t="n">
-        <v>15.34</v>
+        <v>13.98</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -604,154 +600,40 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>VWOB</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Traditional Equity</t>
+          <t>Traditional Bond</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Emerging Markets Bond</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.0009</v>
+        <v>0.002</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0472</v>
+        <v>0.0597</v>
       </c>
       <c r="H5" t="n">
-        <v>23.72</v>
+        <v>11.02</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FLKR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Traditional Equity</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Franklin FTSE South Korea ETF</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Miscellaneous Region</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>0.0009</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.0375</v>
-      </c>
-      <c r="H6" t="n">
-        <v>25.41</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SPEU</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Traditional Equity</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Europe ETF</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Europe Stock</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.0333</v>
-      </c>
-      <c r="H7" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SPEM</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Traditional Equity</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Diversified Emerging Mkts</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.0339</v>
-      </c>
-      <c r="H8" t="n">
-        <v>17.73</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -827,22 +709,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FLIA</t>
+          <t>IAU</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Traditional Bond</t>
+          <t>Metal</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Franklin International Aggregate Bond ETF</t>
+          <t>iShares Gold Trust</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -850,10 +732,10 @@
         <v>0.0025</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1517</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>4.26</v>
+        <v>14.52</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -861,17 +743,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BILS</t>
+          <t>DBMF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Traditional Bond</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
+          <t>iMGP DBi Managed Futures Strategy ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -881,14 +763,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ultrashort Bond</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.00135</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0457</v>
+        <v>0.0781</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -899,37 +781,33 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VCLT</t>
+          <t>MCRO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Traditional Bond</t>
+          <t>Global Macro</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Vanguard Long-Term Corporate Bond Index Fund</t>
+          <t>IQ Hedge Macro Tracker ETF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Long-Term Bond</t>
-        </is>
-      </c>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.0007</v>
+        <v>0.0067</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0535</v>
+        <v>0.025</v>
       </c>
       <c r="H4" t="n">
-        <v>13.98</v>
+        <v>6.59</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -937,37 +815,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VWOB</t>
+          <t>VIXM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Traditional Bond</t>
+          <t>VIX Futures</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Vanguard Emerging Markets Government Bond Index Fund</t>
+          <t>ProShares VIX Mid-Term Futures ETF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NasdaqGM</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Emerging Markets Bond</t>
+          <t>Trading--Miscellaneous</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.002</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0597</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>11.02</v>
+        <v>38.36</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -983,7 +861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1046,17 +924,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IAU</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Metal</t>
+          <t>Traditional Equity</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>iShares Gold Trust</t>
+          <t>Vanguard 500 Index Fund</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1064,15 +942,19 @@
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Large Blend</t>
+        </is>
+      </c>
       <c r="F2" t="n">
-        <v>0.0025</v>
+        <v>0.0004</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.0162</v>
       </c>
       <c r="H2" t="n">
-        <v>14.52</v>
+        <v>18.7</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -1080,17 +962,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DBMF</t>
+          <t>FLCA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Traditional Equity</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>iMGP DBi Managed Futures Strategy ETF</t>
+          <t>Franklin FTSE Canada ETF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1100,17 +982,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.0009</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0781</v>
+        <v>0.0317</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>20.54</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -1118,17 +1000,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MCRO</t>
+          <t>FLJP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Global Macro</t>
+          <t>Traditional Equity</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IQ Hedge Macro Tracker ETF</t>
+          <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1136,15 +1018,19 @@
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Japan Stock</t>
+        </is>
+      </c>
       <c r="F4" t="n">
-        <v>0.0067</v>
+        <v>0.0009</v>
       </c>
       <c r="G4" t="n">
-        <v>0.025</v>
+        <v>0.0224</v>
       </c>
       <c r="H4" t="n">
-        <v>6.59</v>
+        <v>15.34</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -1152,40 +1038,184 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VIXM</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VIX Futures</t>
+          <t>Traditional Equity</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ProShares VIX Mid-Term Futures ETF</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Trading--Miscellaneous</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.009299999999999999</v>
+        <v>0.0009</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.0472</v>
       </c>
       <c r="H5" t="n">
-        <v>38.36</v>
+        <v>23.72</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FLKR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Traditional Equity</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Franklin FTSE South Korea ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Miscellaneous Region</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0375</v>
+      </c>
+      <c r="H6" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPEU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Traditional Equity</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Europe ETF</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Europe Stock</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0007</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="H7" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SPEM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Traditional Equity</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SPDR Portfolio Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Diversified Emerging Mkts</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0007</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0339</v>
+      </c>
+      <c r="H8" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1329.T</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>iShares Core Nikkei 225 ETF</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Tokyo</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0182</v>
+      </c>
+      <c r="H9" t="n">
+        <v>16.89</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix excel_writer.py and excel_reader.py for new structure
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -546,19 +546,19 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>9.779999999999999</v>
+        <v>9.77</v>
       </c>
       <c r="J2" t="n">
-        <v>9.779999999999999</v>
+        <v>9.77</v>
       </c>
       <c r="K2" t="n">
-        <v>12.6</v>
+        <v>12.59</v>
       </c>
       <c r="L2" t="n">
         <v>5.08</v>
       </c>
       <c r="M2" t="n">
-        <v>-10.42</v>
+        <v>-11.15</v>
       </c>
       <c r="N2" t="n">
         <v>0.36</v>
@@ -603,19 +603,19 @@
         <v>7.81</v>
       </c>
       <c r="I3" t="n">
-        <v>1.37</v>
+        <v>1.36</v>
       </c>
       <c r="J3" t="n">
-        <v>9.199999999999999</v>
+        <v>9.19</v>
       </c>
       <c r="K3" t="n">
-        <v>8.23</v>
+        <v>8.24</v>
       </c>
       <c r="L3" t="n">
-        <v>7.09</v>
+        <v>7.11</v>
       </c>
       <c r="M3" t="n">
-        <v>-4.47</v>
+        <v>-4.08</v>
       </c>
       <c r="N3" t="n">
         <v>0.48</v>
@@ -656,19 +656,19 @@
         <v>1.91</v>
       </c>
       <c r="I4" t="n">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="J4" t="n">
-        <v>3.15</v>
+        <v>3.14</v>
       </c>
       <c r="K4" t="n">
-        <v>7.43</v>
+        <v>7.41</v>
       </c>
       <c r="L4" t="n">
         <v>7.49</v>
       </c>
       <c r="M4" t="n">
-        <v>-9.35</v>
+        <v>-8.880000000000001</v>
       </c>
       <c r="N4" t="n">
         <v>-0.28</v>
@@ -713,19 +713,19 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>-8.33</v>
+        <v>-8.41</v>
       </c>
       <c r="J5" t="n">
-        <v>-8.33</v>
+        <v>-8.41</v>
       </c>
       <c r="K5" t="n">
-        <v>45.72</v>
+        <v>45.78</v>
       </c>
       <c r="L5" t="n">
-        <v>26.73</v>
+        <v>26.82</v>
       </c>
       <c r="M5" t="n">
-        <v>-83.34999999999999</v>
+        <v>-83.40000000000001</v>
       </c>
       <c r="N5" t="n">
         <v>-0.3</v>
@@ -770,22 +770,22 @@
         <v>2.38</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.14</v>
+        <v>-0.16</v>
       </c>
       <c r="J6" t="n">
-        <v>2.24</v>
+        <v>2.22</v>
       </c>
       <c r="K6" t="n">
-        <v>6.74</v>
+        <v>6.72</v>
       </c>
       <c r="L6" t="n">
-        <v>7.93</v>
+        <v>7.94</v>
       </c>
       <c r="M6" t="n">
-        <v>-8.83</v>
+        <v>-9.17</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.44</v>
+        <v>-0.45</v>
       </c>
       <c r="O6" t="inlineStr"/>
     </row>
@@ -833,16 +833,16 @@
         <v>1.62</v>
       </c>
       <c r="K7" t="n">
-        <v>5.67</v>
+        <v>5.66</v>
       </c>
       <c r="L7" t="n">
         <v>5.93</v>
       </c>
       <c r="M7" t="n">
-        <v>-7.65</v>
+        <v>-7.72</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.63</v>
+        <v>-0.64</v>
       </c>
       <c r="O7" t="inlineStr"/>
     </row>
@@ -976,7 +976,7 @@
         <v>15.17</v>
       </c>
       <c r="I2" t="n">
-        <v>-3.75</v>
+        <v>-3.76</v>
       </c>
       <c r="J2" t="n">
         <v>11.49</v>
@@ -988,7 +988,7 @@
         <v>12.76</v>
       </c>
       <c r="M2" t="n">
-        <v>-5.77</v>
+        <v>-6.47</v>
       </c>
       <c r="N2" t="n">
         <v>0.59</v>
@@ -1048,7 +1048,7 @@
         <v>3.7</v>
       </c>
       <c r="N3" t="n">
-        <v>-2.86</v>
+        <v>-2.84</v>
       </c>
       <c r="O3" t="inlineStr"/>
     </row>
@@ -1090,19 +1090,19 @@
         <v>5.35</v>
       </c>
       <c r="I4" t="n">
-        <v>-2.22</v>
+        <v>-2.23</v>
       </c>
       <c r="J4" t="n">
-        <v>3.21</v>
+        <v>3.2</v>
       </c>
       <c r="K4" t="n">
         <v>17.61</v>
       </c>
       <c r="L4" t="n">
-        <v>15.64</v>
+        <v>15.65</v>
       </c>
       <c r="M4" t="n">
-        <v>-25.58</v>
+        <v>-26.48</v>
       </c>
       <c r="N4" t="n">
         <v>-0.11</v>
@@ -1159,7 +1159,7 @@
         <v>13.03</v>
       </c>
       <c r="M5" t="n">
-        <v>-16.5</v>
+        <v>-16.53</v>
       </c>
       <c r="N5" t="n">
         <v>-0.25</v>
@@ -1300,19 +1300,19 @@
         <v>1.62</v>
       </c>
       <c r="I2" t="n">
-        <v>12.89</v>
+        <v>12.88</v>
       </c>
       <c r="J2" t="n">
-        <v>14.54</v>
+        <v>14.53</v>
       </c>
       <c r="K2" t="n">
-        <v>20.03</v>
+        <v>20.02</v>
       </c>
       <c r="L2" t="n">
         <v>11.22</v>
       </c>
       <c r="M2" t="n">
-        <v>-18.07</v>
+        <v>-18.46</v>
       </c>
       <c r="N2" t="n">
         <v>0.47</v>
@@ -1357,10 +1357,10 @@
         <v>3.17</v>
       </c>
       <c r="I3" t="n">
-        <v>8.640000000000001</v>
+        <v>8.66</v>
       </c>
       <c r="J3" t="n">
-        <v>11.84</v>
+        <v>11.87</v>
       </c>
       <c r="K3" t="n">
         <v>16.85</v>
@@ -1369,7 +1369,7 @@
         <v>8.77</v>
       </c>
       <c r="M3" t="n">
-        <v>-15.9</v>
+        <v>-15.6</v>
       </c>
       <c r="N3" t="n">
         <v>0.39</v>
@@ -1414,19 +1414,19 @@
         <v>2.24</v>
       </c>
       <c r="I4" t="n">
-        <v>4.16</v>
+        <v>4.18</v>
       </c>
       <c r="J4" t="n">
-        <v>6.42</v>
+        <v>6.44</v>
       </c>
       <c r="K4" t="n">
-        <v>14.66</v>
+        <v>14.68</v>
       </c>
       <c r="L4" t="n">
         <v>10.75</v>
       </c>
       <c r="M4" t="n">
-        <v>-17.97</v>
+        <v>-17.9</v>
       </c>
       <c r="N4" t="n">
         <v>0.08</v>
@@ -1483,7 +1483,7 @@
         <v>7.75</v>
       </c>
       <c r="M5" t="n">
-        <v>-9.529999999999999</v>
+        <v>-9.83</v>
       </c>
       <c r="N5" t="n">
         <v>0.31</v>
@@ -1528,22 +1528,22 @@
         <v>3.75</v>
       </c>
       <c r="I6" t="n">
-        <v>1.34</v>
+        <v>1.37</v>
       </c>
       <c r="J6" t="n">
-        <v>5.2</v>
+        <v>5.23</v>
       </c>
       <c r="K6" t="n">
-        <v>26.9</v>
+        <v>26.91</v>
       </c>
       <c r="L6" t="n">
         <v>17.31</v>
       </c>
       <c r="M6" t="n">
-        <v>-39.1</v>
+        <v>-39.16</v>
       </c>
       <c r="N6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="O6" t="inlineStr"/>
     </row>
@@ -1585,22 +1585,22 @@
         <v>3.33</v>
       </c>
       <c r="I7" t="n">
-        <v>5.36</v>
+        <v>5.37</v>
       </c>
       <c r="J7" t="n">
         <v>8.73</v>
       </c>
       <c r="K7" t="n">
-        <v>15.63</v>
+        <v>15.64</v>
       </c>
       <c r="L7" t="n">
-        <v>10.69</v>
+        <v>10.7</v>
       </c>
       <c r="M7" t="n">
-        <v>-16.36</v>
+        <v>-16.91</v>
       </c>
       <c r="N7" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="O7" t="inlineStr"/>
     </row>
@@ -1642,10 +1642,10 @@
         <v>3.39</v>
       </c>
       <c r="I8" t="n">
-        <v>1.53</v>
+        <v>1.52</v>
       </c>
       <c r="J8" t="n">
-        <v>4.95</v>
+        <v>4.94</v>
       </c>
       <c r="K8" t="n">
         <v>14.52</v>
@@ -1654,7 +1654,7 @@
         <v>11.87</v>
       </c>
       <c r="M8" t="n">
-        <v>-19.43</v>
+        <v>-18.98</v>
       </c>
       <c r="N8" t="n">
         <v>-0.02</v>
@@ -1699,19 +1699,19 @@
         <v>5.41</v>
       </c>
       <c r="I9" t="n">
-        <v>-6.34</v>
+        <v>-6.32</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.88</v>
+        <v>-0.86</v>
       </c>
       <c r="K9" t="n">
         <v>13.82</v>
       </c>
       <c r="L9" t="n">
-        <v>16.22</v>
+        <v>16.21</v>
       </c>
       <c r="M9" t="n">
-        <v>-23.59</v>
+        <v>-23.3</v>
       </c>
       <c r="N9" t="n">
         <v>-0.44</v>
@@ -1756,19 +1756,19 @@
         <v>4.92</v>
       </c>
       <c r="I10" t="n">
-        <v>2.51</v>
+        <v>2.46</v>
       </c>
       <c r="J10" t="n">
-        <v>7.56</v>
+        <v>7.52</v>
       </c>
       <c r="K10" t="n">
-        <v>26.29</v>
+        <v>26.3</v>
       </c>
       <c r="L10" t="n">
-        <v>16.47</v>
+        <v>16.48</v>
       </c>
       <c r="M10" t="n">
-        <v>-35.96</v>
+        <v>-35.98</v>
       </c>
       <c r="N10" t="n">
         <v>0.09</v>
@@ -1813,19 +1813,19 @@
         <v>12.91</v>
       </c>
       <c r="I11" t="n">
-        <v>-1.12</v>
+        <v>-1.13</v>
       </c>
       <c r="J11" t="n">
-        <v>11.82</v>
+        <v>11.8</v>
       </c>
       <c r="K11" t="n">
         <v>7.83</v>
       </c>
       <c r="L11" t="n">
-        <v>9.039999999999999</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="M11" t="n">
-        <v>-1.06</v>
+        <v>-0.97</v>
       </c>
       <c r="N11" t="n">
         <v>0.84</v>

</xml_diff>

<commit_message>
add sub category risk weight add risk weight validation
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,65 +448,70 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Sub Category Risk Weight</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Category Name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Exchange Name</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Traded Currency</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Expense Ratio</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Simple Return</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Total Return</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Standard Deviation</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Downside Deviation</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Value at Risk 95%</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Sharpe Ratio</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Asset Weight</t>
         </is>
@@ -523,47 +528,50 @@
           <t>Metal</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>iShares Gold Trust</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.25</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="n">
-        <v>9.77</v>
-      </c>
       <c r="J2" t="n">
-        <v>9.77</v>
+        <v>9.779999999999999</v>
       </c>
       <c r="K2" t="n">
-        <v>12.59</v>
+        <v>9.779999999999999</v>
       </c>
       <c r="L2" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="M2" t="n">
         <v>5.08</v>
       </c>
-      <c r="M2" t="n">
-        <v>-11.15</v>
-      </c>
       <c r="N2" t="n">
+        <v>-10.32</v>
+      </c>
+      <c r="O2" t="n">
         <v>0.36</v>
       </c>
-      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -576,51 +584,54 @@
           <t>Managed Futures</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>iMGP DBi Managed Futures Strategy ETF</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Managed Futures</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.85</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>7.81</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>1.36</v>
       </c>
-      <c r="J3" t="n">
-        <v>9.19</v>
-      </c>
       <c r="K3" t="n">
-        <v>8.24</v>
+        <v>9.18</v>
       </c>
       <c r="L3" t="n">
-        <v>7.11</v>
+        <v>8.25</v>
       </c>
       <c r="M3" t="n">
-        <v>-4.08</v>
+        <v>7.13</v>
       </c>
       <c r="N3" t="n">
+        <v>-4.53</v>
+      </c>
+      <c r="O3" t="n">
         <v>0.48</v>
       </c>
-      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -633,47 +644,50 @@
           <t>Global Macro</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>IQ Hedge Multi-Strategy Tracker ETF</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.78</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>1.91</v>
       </c>
-      <c r="I4" t="n">
-        <v>1.23</v>
-      </c>
       <c r="J4" t="n">
-        <v>3.14</v>
+        <v>1.25</v>
       </c>
       <c r="K4" t="n">
-        <v>7.41</v>
+        <v>3.17</v>
       </c>
       <c r="L4" t="n">
+        <v>7.45</v>
+      </c>
+      <c r="M4" t="n">
         <v>7.49</v>
       </c>
-      <c r="M4" t="n">
-        <v>-8.880000000000001</v>
-      </c>
       <c r="N4" t="n">
+        <v>-9.18</v>
+      </c>
+      <c r="O4" t="n">
         <v>-0.28</v>
       </c>
-      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -686,51 +700,54 @@
           <t>VIX Futures</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>ProShares VIX Mid-Term Futures ETF</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Trading--Miscellaneous</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Cboe US</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0.93</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="I5" t="n">
-        <v>-8.41</v>
-      </c>
       <c r="J5" t="n">
-        <v>-8.41</v>
+        <v>-8.380000000000001</v>
       </c>
       <c r="K5" t="n">
-        <v>45.78</v>
+        <v>-8.380000000000001</v>
       </c>
       <c r="L5" t="n">
-        <v>26.82</v>
+        <v>45.76</v>
       </c>
       <c r="M5" t="n">
-        <v>-83.40000000000001</v>
+        <v>26.79</v>
       </c>
       <c r="N5" t="n">
+        <v>-84.04000000000001</v>
+      </c>
+      <c r="O5" t="n">
         <v>-0.3</v>
       </c>
-      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -743,51 +760,54 @@
           <t>Currency</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>Invesco CurrencyShares British Pound Sterling Trust</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Single Currency</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>0.4</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>2.38</v>
       </c>
-      <c r="I6" t="n">
-        <v>-0.16</v>
-      </c>
       <c r="J6" t="n">
-        <v>2.22</v>
+        <v>-0.14</v>
       </c>
       <c r="K6" t="n">
-        <v>6.72</v>
+        <v>2.24</v>
       </c>
       <c r="L6" t="n">
+        <v>6.74</v>
+      </c>
+      <c r="M6" t="n">
         <v>7.94</v>
       </c>
-      <c r="M6" t="n">
-        <v>-9.17</v>
-      </c>
       <c r="N6" t="n">
-        <v>-0.45</v>
-      </c>
-      <c r="O6" t="inlineStr"/>
+        <v>-8.69</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-0.44</v>
+      </c>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -800,51 +820,54 @@
           <t>Currency</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>50</v>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>Invesco CurrencyShares Swiss Franc Trust</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Single Currency</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.4</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>0</v>
       </c>
-      <c r="I7" t="n">
-        <v>1.62</v>
-      </c>
       <c r="J7" t="n">
-        <v>1.62</v>
+        <v>1.6</v>
       </c>
       <c r="K7" t="n">
-        <v>5.66</v>
+        <v>1.6</v>
       </c>
       <c r="L7" t="n">
+        <v>5.64</v>
+      </c>
+      <c r="M7" t="n">
         <v>5.93</v>
       </c>
-      <c r="M7" t="n">
-        <v>-7.72</v>
-      </c>
       <c r="N7" t="n">
+        <v>-7.87</v>
+      </c>
+      <c r="O7" t="n">
         <v>-0.64</v>
       </c>
-      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -857,7 +880,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -878,65 +901,70 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Sub Category Risk Weight</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Category Name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Exchange Name</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Traded Currency</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Expense Ratio</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Simple Return</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Total Return</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Standard Deviation</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Downside Deviation</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Value at Risk 95%</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Sharpe Ratio</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Asset Weight</t>
         </is>
@@ -953,47 +981,50 @@
           <t>Traditional Bond</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>56.25</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>Franklin International Aggregate Bond ETF</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
         <is>
           <t>Cboe US</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.25</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>15.17</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>-3.76</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>11.49</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>10.68</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>12.76</v>
       </c>
-      <c r="M2" t="n">
-        <v>-6.47</v>
-      </c>
       <c r="N2" t="n">
+        <v>-6.06</v>
+      </c>
+      <c r="O2" t="n">
         <v>0.59</v>
       </c>
-      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1006,51 +1037,54 @@
           <t>Traditional Bond</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>9.380000000000001</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>SPDR Bloomberg 3-12 Month T-Bill ETF</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Ultrashort Bond</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.135</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>4.57</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>-0.32</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>4.25</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.34</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>5.54</v>
       </c>
-      <c r="M3" t="n">
-        <v>3.7</v>
-      </c>
       <c r="N3" t="n">
-        <v>-2.84</v>
-      </c>
-      <c r="O3" t="inlineStr"/>
+        <v>3.69</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-2.85</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1063,51 +1097,54 @@
           <t>Traditional Bond</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>9.380000000000001</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>Vanguard Long-Term Corporate Bond Index Fund</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Long-Term Bond</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>NasdaqGM</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>5.35</v>
       </c>
-      <c r="I4" t="n">
-        <v>-2.23</v>
-      </c>
       <c r="J4" t="n">
-        <v>3.2</v>
+        <v>-2.2</v>
       </c>
       <c r="K4" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="L4" t="n">
         <v>17.61</v>
       </c>
-      <c r="L4" t="n">
-        <v>15.65</v>
-      </c>
       <c r="M4" t="n">
-        <v>-26.48</v>
+        <v>15.64</v>
       </c>
       <c r="N4" t="n">
+        <v>-25.66</v>
+      </c>
+      <c r="O4" t="n">
         <v>-0.11</v>
       </c>
-      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1120,51 +1157,54 @@
           <t>Traditional Bond</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>Vanguard Emerging Markets Government Bond Index Fund</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Emerging Markets Bond</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>NasdaqGM</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0.2</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>5.97</v>
       </c>
-      <c r="I5" t="n">
-        <v>-3.68</v>
-      </c>
       <c r="J5" t="n">
-        <v>2.32</v>
+        <v>-3.65</v>
       </c>
       <c r="K5" t="n">
-        <v>11.38</v>
+        <v>2.35</v>
       </c>
       <c r="L5" t="n">
-        <v>13.03</v>
+        <v>11.4</v>
       </c>
       <c r="M5" t="n">
-        <v>-16.53</v>
+        <v>13.02</v>
       </c>
       <c r="N5" t="n">
+        <v>-16.3</v>
+      </c>
+      <c r="O5" t="n">
         <v>-0.25</v>
       </c>
-      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1177,7 +1217,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1198,65 +1238,70 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Sub Category Risk Weight</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Category Name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Exchange Name</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Traded Currency</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Expense Ratio</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Simple Return</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Total Return</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Standard Deviation</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Downside Deviation</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Value at Risk 95%</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Sharpe Ratio</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Asset Weight</t>
         </is>
@@ -1273,51 +1318,54 @@
           <t>Traditional Equity</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>Vanguard 500 Index Fund</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Large Blend</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.04</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>1.62</v>
       </c>
-      <c r="I2" t="n">
-        <v>12.88</v>
-      </c>
       <c r="J2" t="n">
-        <v>14.53</v>
+        <v>12.9</v>
       </c>
       <c r="K2" t="n">
-        <v>20.02</v>
+        <v>14.55</v>
       </c>
       <c r="L2" t="n">
+        <v>20.03</v>
+      </c>
+      <c r="M2" t="n">
         <v>11.22</v>
       </c>
-      <c r="M2" t="n">
-        <v>-18.46</v>
-      </c>
       <c r="N2" t="n">
+        <v>-18.49</v>
+      </c>
+      <c r="O2" t="n">
         <v>0.47</v>
       </c>
-      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1330,51 +1378,54 @@
           <t>Traditional Equity</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>Franklin FTSE Canada ETF</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Miscellaneous Region</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.09</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>3.17</v>
       </c>
-      <c r="I3" t="n">
-        <v>8.66</v>
-      </c>
       <c r="J3" t="n">
-        <v>11.87</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>16.85</v>
+        <v>11.91</v>
       </c>
       <c r="L3" t="n">
+        <v>16.84</v>
+      </c>
+      <c r="M3" t="n">
         <v>8.77</v>
       </c>
-      <c r="M3" t="n">
-        <v>-15.6</v>
-      </c>
       <c r="N3" t="n">
-        <v>0.39</v>
-      </c>
-      <c r="O3" t="inlineStr"/>
+        <v>-15.74</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1387,51 +1438,54 @@
           <t>Traditional Equity</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>Franklin FTSE Japan ETF</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Japan Stock</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.09</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>2.24</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>4.18</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>6.44</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>14.68</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>10.75</v>
       </c>
-      <c r="M4" t="n">
-        <v>-17.9</v>
-      </c>
       <c r="N4" t="n">
+        <v>-17.88</v>
+      </c>
+      <c r="O4" t="n">
         <v>0.08</v>
       </c>
-      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1444,51 +1498,54 @@
           <t>Traditional Equity</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Miscellaneous Region</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0.09</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>4.72</v>
       </c>
-      <c r="I5" t="n">
-        <v>3.86</v>
-      </c>
       <c r="J5" t="n">
-        <v>8.6</v>
+        <v>4.06</v>
       </c>
       <c r="K5" t="n">
-        <v>11.02</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="L5" t="n">
-        <v>7.75</v>
+        <v>10.98</v>
       </c>
       <c r="M5" t="n">
-        <v>-9.83</v>
+        <v>7.68</v>
       </c>
       <c r="N5" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="O5" t="inlineStr"/>
+        <v>-9.039999999999999</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1501,51 +1558,54 @@
           <t>Traditional Equity</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>Franklin FTSE South Korea ETF</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Miscellaneous Region</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>0.09</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>3.75</v>
       </c>
-      <c r="I6" t="n">
-        <v>1.37</v>
-      </c>
       <c r="J6" t="n">
-        <v>5.23</v>
+        <v>1.4</v>
       </c>
       <c r="K6" t="n">
-        <v>26.91</v>
+        <v>5.25</v>
       </c>
       <c r="L6" t="n">
+        <v>26.92</v>
+      </c>
+      <c r="M6" t="n">
         <v>17.31</v>
       </c>
-      <c r="M6" t="n">
-        <v>-39.16</v>
-      </c>
       <c r="N6" t="n">
+        <v>-38.53</v>
+      </c>
+      <c r="O6" t="n">
         <v>0</v>
       </c>
-      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1558,51 +1618,54 @@
           <t>Traditional Equity</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>24.75</v>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>SPDR Portfolio Europe ETF</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Europe Stock</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>3.33</v>
       </c>
-      <c r="I7" t="n">
-        <v>5.37</v>
-      </c>
       <c r="J7" t="n">
-        <v>8.73</v>
+        <v>5.34</v>
       </c>
       <c r="K7" t="n">
-        <v>15.64</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="L7" t="n">
+        <v>15.62</v>
+      </c>
+      <c r="M7" t="n">
         <v>10.7</v>
       </c>
-      <c r="M7" t="n">
-        <v>-16.91</v>
-      </c>
       <c r="N7" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="O7" t="inlineStr"/>
+        <v>-16.8</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1615,51 +1678,54 @@
           <t>Traditional Equity</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>25.74</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>SPDR Portfolio Emerging Markets ETF</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Diversified Emerging Mkts</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>3.39</v>
       </c>
-      <c r="I8" t="n">
-        <v>1.52</v>
-      </c>
       <c r="J8" t="n">
-        <v>4.94</v>
+        <v>1.54</v>
       </c>
       <c r="K8" t="n">
-        <v>14.52</v>
+        <v>4.96</v>
       </c>
       <c r="L8" t="n">
+        <v>14.53</v>
+      </c>
+      <c r="M8" t="n">
         <v>11.87</v>
       </c>
-      <c r="M8" t="n">
-        <v>-18.98</v>
-      </c>
       <c r="N8" t="n">
+        <v>-19.09</v>
+      </c>
+      <c r="O8" t="n">
         <v>-0.02</v>
       </c>
-      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1672,51 +1738,54 @@
           <t>REIT</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>50</v>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>SPDR Dow Jones International Real Estate ETF</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Global Real Estate</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>0.59</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>5.41</v>
       </c>
-      <c r="I9" t="n">
-        <v>-6.32</v>
-      </c>
       <c r="J9" t="n">
-        <v>-0.86</v>
+        <v>-6.33</v>
       </c>
       <c r="K9" t="n">
+        <v>-0.88</v>
+      </c>
+      <c r="L9" t="n">
         <v>13.82</v>
       </c>
-      <c r="L9" t="n">
-        <v>16.21</v>
-      </c>
       <c r="M9" t="n">
-        <v>-23.3</v>
+        <v>16.22</v>
       </c>
       <c r="N9" t="n">
+        <v>-23.51</v>
+      </c>
+      <c r="O9" t="n">
         <v>-0.44</v>
       </c>
-      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1729,51 +1798,54 @@
           <t>REIT</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" t="n">
+        <v>50</v>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>Vanguard Real Estate Index Fund</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Real Estate</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>NYSEArca</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>0.1</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>4.92</v>
       </c>
-      <c r="I10" t="n">
-        <v>2.46</v>
-      </c>
       <c r="J10" t="n">
-        <v>7.52</v>
+        <v>2.57</v>
       </c>
       <c r="K10" t="n">
-        <v>26.3</v>
+        <v>7.62</v>
       </c>
       <c r="L10" t="n">
-        <v>16.48</v>
+        <v>26.28</v>
       </c>
       <c r="M10" t="n">
-        <v>-35.98</v>
+        <v>16.46</v>
       </c>
       <c r="N10" t="n">
+        <v>-35.5</v>
+      </c>
+      <c r="O10" t="n">
         <v>0.09</v>
       </c>
-      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1786,51 +1858,54 @@
           <t>Commodity</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>Invesco Optimum Yield Diversified Commodity Strategy No K-1 ETF</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Commodities Broad Basket</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>NasdaqGM</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>0.59</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>12.91</v>
       </c>
-      <c r="I11" t="n">
-        <v>-1.13</v>
-      </c>
       <c r="J11" t="n">
+        <v>-1.14</v>
+      </c>
+      <c r="K11" t="n">
         <v>11.8</v>
       </c>
-      <c r="K11" t="n">
-        <v>7.83</v>
-      </c>
       <c r="L11" t="n">
-        <v>9.050000000000001</v>
+        <v>7.84</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.97</v>
+        <v>9.06</v>
       </c>
       <c r="N11" t="n">
+        <v>-1.07</v>
+      </c>
+      <c r="O11" t="n">
         <v>0.84</v>
       </c>
-      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add risk weight to asset weight calculation
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -554,22 +554,22 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>9.779999999999999</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="K2" t="n">
-        <v>9.779999999999999</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="L2" t="n">
-        <v>12.6</v>
+        <v>12.28</v>
       </c>
       <c r="M2" t="n">
-        <v>5.08</v>
+        <v>4.83</v>
       </c>
       <c r="N2" t="n">
-        <v>-10.32</v>
+        <v>-10.22</v>
       </c>
       <c r="O2" t="n">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="P2" t="inlineStr"/>
     </row>
@@ -614,22 +614,22 @@
         <v>7.81</v>
       </c>
       <c r="J3" t="n">
-        <v>1.36</v>
+        <v>1.53</v>
       </c>
       <c r="K3" t="n">
-        <v>9.18</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>8.25</v>
+        <v>8.380000000000001</v>
       </c>
       <c r="M3" t="n">
-        <v>7.13</v>
+        <v>7.06</v>
       </c>
       <c r="N3" t="n">
-        <v>-4.53</v>
+        <v>-4.06</v>
       </c>
       <c r="O3" t="n">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="P3" t="inlineStr"/>
     </row>
@@ -670,22 +670,22 @@
         <v>1.91</v>
       </c>
       <c r="J4" t="n">
-        <v>1.25</v>
+        <v>1.26</v>
       </c>
       <c r="K4" t="n">
-        <v>3.17</v>
+        <v>3.18</v>
       </c>
       <c r="L4" t="n">
-        <v>7.45</v>
+        <v>7.44</v>
       </c>
       <c r="M4" t="n">
         <v>7.49</v>
       </c>
       <c r="N4" t="n">
-        <v>-9.18</v>
+        <v>-9.039999999999999</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.28</v>
+        <v>-0.27</v>
       </c>
       <c r="P4" t="inlineStr"/>
     </row>
@@ -730,22 +730,22 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>-8.380000000000001</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="K5" t="n">
-        <v>-8.380000000000001</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="L5" t="n">
-        <v>45.76</v>
+        <v>44.19</v>
       </c>
       <c r="M5" t="n">
-        <v>26.79</v>
+        <v>26.64</v>
       </c>
       <c r="N5" t="n">
-        <v>-84.04000000000001</v>
+        <v>-82.28</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.3</v>
+        <v>-0.31</v>
       </c>
       <c r="P5" t="inlineStr"/>
     </row>
@@ -790,22 +790,22 @@
         <v>2.38</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.14</v>
+        <v>-0.25</v>
       </c>
       <c r="K6" t="n">
-        <v>2.24</v>
+        <v>2.13</v>
       </c>
       <c r="L6" t="n">
-        <v>6.74</v>
+        <v>6.54</v>
       </c>
       <c r="M6" t="n">
-        <v>7.94</v>
+        <v>7.88</v>
       </c>
       <c r="N6" t="n">
-        <v>-8.69</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.44</v>
+        <v>-0.47</v>
       </c>
       <c r="P6" t="inlineStr"/>
     </row>
@@ -850,22 +850,22 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>1.6</v>
+        <v>1.52</v>
       </c>
       <c r="K7" t="n">
-        <v>1.6</v>
+        <v>1.52</v>
       </c>
       <c r="L7" t="n">
-        <v>5.64</v>
+        <v>5.42</v>
       </c>
       <c r="M7" t="n">
-        <v>5.93</v>
+        <v>5.85</v>
       </c>
       <c r="N7" t="n">
-        <v>-7.87</v>
+        <v>-7.34</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.64</v>
+        <v>-0.68</v>
       </c>
       <c r="P7" t="inlineStr"/>
     </row>
@@ -1007,22 +1007,22 @@
         <v>15.17</v>
       </c>
       <c r="J2" t="n">
-        <v>-3.76</v>
+        <v>-3.74</v>
       </c>
       <c r="K2" t="n">
-        <v>11.49</v>
+        <v>11.5</v>
       </c>
       <c r="L2" t="n">
-        <v>10.68</v>
+        <v>10.81</v>
       </c>
       <c r="M2" t="n">
-        <v>12.76</v>
+        <v>12.83</v>
       </c>
       <c r="N2" t="n">
-        <v>-6.06</v>
+        <v>-6.38</v>
       </c>
       <c r="O2" t="n">
-        <v>0.59</v>
+        <v>0.58</v>
       </c>
       <c r="P2" t="inlineStr"/>
     </row>
@@ -1079,10 +1079,10 @@
         <v>5.54</v>
       </c>
       <c r="N3" t="n">
-        <v>3.69</v>
+        <v>3.7</v>
       </c>
       <c r="O3" t="n">
-        <v>-2.85</v>
+        <v>-2.84</v>
       </c>
       <c r="P3" t="inlineStr"/>
     </row>
@@ -1127,19 +1127,19 @@
         <v>5.35</v>
       </c>
       <c r="J4" t="n">
-        <v>-2.2</v>
+        <v>-2.15</v>
       </c>
       <c r="K4" t="n">
-        <v>3.23</v>
+        <v>3.28</v>
       </c>
       <c r="L4" t="n">
-        <v>17.61</v>
+        <v>17.89</v>
       </c>
       <c r="M4" t="n">
-        <v>15.64</v>
+        <v>15.8</v>
       </c>
       <c r="N4" t="n">
-        <v>-25.66</v>
+        <v>-26.26</v>
       </c>
       <c r="O4" t="n">
         <v>-0.11</v>
@@ -1187,19 +1187,19 @@
         <v>5.97</v>
       </c>
       <c r="J5" t="n">
-        <v>-3.65</v>
+        <v>-3.63</v>
       </c>
       <c r="K5" t="n">
-        <v>2.35</v>
+        <v>2.38</v>
       </c>
       <c r="L5" t="n">
-        <v>11.4</v>
+        <v>11.56</v>
       </c>
       <c r="M5" t="n">
-        <v>13.02</v>
+        <v>13.11</v>
       </c>
       <c r="N5" t="n">
-        <v>-16.3</v>
+        <v>-16.61</v>
       </c>
       <c r="O5" t="n">
         <v>-0.25</v>
@@ -1348,19 +1348,19 @@
         <v>1.62</v>
       </c>
       <c r="J2" t="n">
-        <v>12.9</v>
+        <v>12.92</v>
       </c>
       <c r="K2" t="n">
-        <v>14.55</v>
+        <v>14.56</v>
       </c>
       <c r="L2" t="n">
-        <v>20.03</v>
+        <v>19.75</v>
       </c>
       <c r="M2" t="n">
-        <v>11.22</v>
+        <v>11.12</v>
       </c>
       <c r="N2" t="n">
-        <v>-18.49</v>
+        <v>-17.39</v>
       </c>
       <c r="O2" t="n">
         <v>0.47</v>
@@ -1408,19 +1408,19 @@
         <v>3.17</v>
       </c>
       <c r="J3" t="n">
-        <v>8.699999999999999</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>11.91</v>
+        <v>11.98</v>
       </c>
       <c r="L3" t="n">
-        <v>16.84</v>
+        <v>16.71</v>
       </c>
       <c r="M3" t="n">
-        <v>8.77</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="N3" t="n">
-        <v>-15.74</v>
+        <v>-15.37</v>
       </c>
       <c r="O3" t="n">
         <v>0.4</v>
@@ -1468,22 +1468,22 @@
         <v>2.24</v>
       </c>
       <c r="J4" t="n">
-        <v>4.18</v>
+        <v>4.22</v>
       </c>
       <c r="K4" t="n">
-        <v>6.44</v>
+        <v>6.48</v>
       </c>
       <c r="L4" t="n">
-        <v>14.68</v>
+        <v>14.83</v>
       </c>
       <c r="M4" t="n">
-        <v>10.75</v>
+        <v>10.84</v>
       </c>
       <c r="N4" t="n">
-        <v>-17.88</v>
+        <v>-17.65</v>
       </c>
       <c r="O4" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="P4" t="inlineStr"/>
     </row>
@@ -1528,19 +1528,19 @@
         <v>4.72</v>
       </c>
       <c r="J5" t="n">
-        <v>4.06</v>
+        <v>4</v>
       </c>
       <c r="K5" t="n">
-        <v>8.800000000000001</v>
+        <v>8.74</v>
       </c>
       <c r="L5" t="n">
-        <v>10.98</v>
+        <v>10.64</v>
       </c>
       <c r="M5" t="n">
-        <v>7.68</v>
+        <v>7.52</v>
       </c>
       <c r="N5" t="n">
-        <v>-9.039999999999999</v>
+        <v>-8.779999999999999</v>
       </c>
       <c r="O5" t="n">
         <v>0.33</v>
@@ -1588,22 +1588,22 @@
         <v>3.75</v>
       </c>
       <c r="J6" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="K6" t="n">
-        <v>5.25</v>
+        <v>5.15</v>
       </c>
       <c r="L6" t="n">
-        <v>26.92</v>
+        <v>26.45</v>
       </c>
       <c r="M6" t="n">
-        <v>17.31</v>
+        <v>17.11</v>
       </c>
       <c r="N6" t="n">
-        <v>-38.53</v>
+        <v>-39.36</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="P6" t="inlineStr"/>
     </row>
@@ -1648,22 +1648,22 @@
         <v>3.33</v>
       </c>
       <c r="J7" t="n">
-        <v>5.34</v>
+        <v>5.31</v>
       </c>
       <c r="K7" t="n">
-        <v>8.699999999999999</v>
+        <v>8.67</v>
       </c>
       <c r="L7" t="n">
-        <v>15.62</v>
+        <v>15.35</v>
       </c>
       <c r="M7" t="n">
-        <v>10.7</v>
+        <v>10.65</v>
       </c>
       <c r="N7" t="n">
-        <v>-16.8</v>
+        <v>-16.25</v>
       </c>
       <c r="O7" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="P7" t="inlineStr"/>
     </row>
@@ -1708,19 +1708,19 @@
         <v>3.39</v>
       </c>
       <c r="J8" t="n">
-        <v>1.54</v>
+        <v>1.58</v>
       </c>
       <c r="K8" t="n">
-        <v>4.96</v>
+        <v>5</v>
       </c>
       <c r="L8" t="n">
-        <v>14.53</v>
+        <v>14.48</v>
       </c>
       <c r="M8" t="n">
-        <v>11.87</v>
+        <v>11.9</v>
       </c>
       <c r="N8" t="n">
-        <v>-19.09</v>
+        <v>-19.05</v>
       </c>
       <c r="O8" t="n">
         <v>-0.02</v>
@@ -1774,16 +1774,16 @@
         <v>-0.88</v>
       </c>
       <c r="L9" t="n">
-        <v>13.82</v>
+        <v>13.66</v>
       </c>
       <c r="M9" t="n">
-        <v>16.22</v>
+        <v>16.13</v>
       </c>
       <c r="N9" t="n">
-        <v>-23.51</v>
+        <v>-23.6</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.44</v>
+        <v>-0.45</v>
       </c>
       <c r="P9" t="inlineStr"/>
     </row>
@@ -1828,22 +1828,22 @@
         <v>4.92</v>
       </c>
       <c r="J10" t="n">
-        <v>2.57</v>
+        <v>2.35</v>
       </c>
       <c r="K10" t="n">
-        <v>7.62</v>
+        <v>7.4</v>
       </c>
       <c r="L10" t="n">
-        <v>26.28</v>
+        <v>26.07</v>
       </c>
       <c r="M10" t="n">
-        <v>16.46</v>
+        <v>16.52</v>
       </c>
       <c r="N10" t="n">
-        <v>-35.5</v>
+        <v>-35.76</v>
       </c>
       <c r="O10" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="P10" t="inlineStr"/>
     </row>
@@ -1888,22 +1888,22 @@
         <v>12.91</v>
       </c>
       <c r="J11" t="n">
-        <v>-1.14</v>
+        <v>-1.11</v>
       </c>
       <c r="K11" t="n">
-        <v>11.8</v>
+        <v>11.83</v>
       </c>
       <c r="L11" t="n">
-        <v>7.84</v>
+        <v>7.96</v>
       </c>
       <c r="M11" t="n">
-        <v>9.06</v>
+        <v>9.119999999999999</v>
       </c>
       <c r="N11" t="n">
-        <v>-1.07</v>
+        <v>-1.36</v>
       </c>
       <c r="O11" t="n">
-        <v>0.84</v>
+        <v>0.83</v>
       </c>
       <c r="P11" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
add sub category aggregated returns in series with K-NN filling method
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -566,7 +566,7 @@
         <v>4.83</v>
       </c>
       <c r="N2" t="n">
-        <v>-10.22</v>
+        <v>-10.5</v>
       </c>
       <c r="O2" t="n">
         <v>0.37</v>
@@ -626,7 +626,7 @@
         <v>7.06</v>
       </c>
       <c r="N3" t="n">
-        <v>-4.06</v>
+        <v>-4.51</v>
       </c>
       <c r="O3" t="n">
         <v>0.49</v>
@@ -682,7 +682,7 @@
         <v>7.49</v>
       </c>
       <c r="N4" t="n">
-        <v>-9.039999999999999</v>
+        <v>-9.369999999999999</v>
       </c>
       <c r="O4" t="n">
         <v>-0.27</v>
@@ -742,7 +742,7 @@
         <v>26.64</v>
       </c>
       <c r="N5" t="n">
-        <v>-82.28</v>
+        <v>-81.81</v>
       </c>
       <c r="O5" t="n">
         <v>-0.31</v>
@@ -802,7 +802,7 @@
         <v>7.88</v>
       </c>
       <c r="N6" t="n">
-        <v>-8.550000000000001</v>
+        <v>-8.84</v>
       </c>
       <c r="O6" t="n">
         <v>-0.47</v>
@@ -862,7 +862,7 @@
         <v>5.85</v>
       </c>
       <c r="N7" t="n">
-        <v>-7.34</v>
+        <v>-7.24</v>
       </c>
       <c r="O7" t="n">
         <v>-0.68</v>
@@ -1019,7 +1019,7 @@
         <v>12.83</v>
       </c>
       <c r="N2" t="n">
-        <v>-6.38</v>
+        <v>-5.88</v>
       </c>
       <c r="O2" t="n">
         <v>0.58</v>
@@ -1079,7 +1079,7 @@
         <v>5.54</v>
       </c>
       <c r="N3" t="n">
-        <v>3.7</v>
+        <v>3.68</v>
       </c>
       <c r="O3" t="n">
         <v>-2.84</v>
@@ -1139,7 +1139,7 @@
         <v>15.8</v>
       </c>
       <c r="N4" t="n">
-        <v>-26.26</v>
+        <v>-27.15</v>
       </c>
       <c r="O4" t="n">
         <v>-0.11</v>
@@ -1199,7 +1199,7 @@
         <v>13.11</v>
       </c>
       <c r="N5" t="n">
-        <v>-16.61</v>
+        <v>-16.35</v>
       </c>
       <c r="O5" t="n">
         <v>-0.25</v>
@@ -1360,7 +1360,7 @@
         <v>11.12</v>
       </c>
       <c r="N2" t="n">
-        <v>-17.39</v>
+        <v>-17.9</v>
       </c>
       <c r="O2" t="n">
         <v>0.47</v>
@@ -1420,7 +1420,7 @@
         <v>8.640000000000001</v>
       </c>
       <c r="N3" t="n">
-        <v>-15.37</v>
+        <v>-15.32</v>
       </c>
       <c r="O3" t="n">
         <v>0.4</v>
@@ -1480,7 +1480,7 @@
         <v>10.84</v>
       </c>
       <c r="N4" t="n">
-        <v>-17.65</v>
+        <v>-18.54</v>
       </c>
       <c r="O4" t="n">
         <v>0.09</v>
@@ -1540,7 +1540,7 @@
         <v>7.52</v>
       </c>
       <c r="N5" t="n">
-        <v>-8.779999999999999</v>
+        <v>-8.81</v>
       </c>
       <c r="O5" t="n">
         <v>0.33</v>
@@ -1600,7 +1600,7 @@
         <v>17.11</v>
       </c>
       <c r="N6" t="n">
-        <v>-39.36</v>
+        <v>-38.25</v>
       </c>
       <c r="O6" t="n">
         <v>-0</v>
@@ -1660,7 +1660,7 @@
         <v>10.65</v>
       </c>
       <c r="N7" t="n">
-        <v>-16.25</v>
+        <v>-16.35</v>
       </c>
       <c r="O7" t="n">
         <v>0.23</v>
@@ -1720,7 +1720,7 @@
         <v>11.9</v>
       </c>
       <c r="N8" t="n">
-        <v>-19.05</v>
+        <v>-18.73</v>
       </c>
       <c r="O8" t="n">
         <v>-0.02</v>
@@ -1780,7 +1780,7 @@
         <v>16.13</v>
       </c>
       <c r="N9" t="n">
-        <v>-23.6</v>
+        <v>-23.04</v>
       </c>
       <c r="O9" t="n">
         <v>-0.45</v>
@@ -1840,7 +1840,7 @@
         <v>16.52</v>
       </c>
       <c r="N10" t="n">
-        <v>-35.76</v>
+        <v>-35.3</v>
       </c>
       <c r="O10" t="n">
         <v>0.08</v>
@@ -1900,7 +1900,7 @@
         <v>9.119999999999999</v>
       </c>
       <c r="N11" t="n">
-        <v>-1.36</v>
+        <v>-1.52</v>
       </c>
       <c r="O11" t="n">
         <v>0.83</v>

</xml_diff>

<commit_message>
add mean_variance_optimizer.py expected_returns and correlation, covariance calculation with returns in series add sub category optimization and aggregate data
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -566,7 +566,7 @@
         <v>4.83</v>
       </c>
       <c r="N2" t="n">
-        <v>-10.5</v>
+        <v>-10.43</v>
       </c>
       <c r="O2" t="n">
         <v>0.37</v>
@@ -626,7 +626,7 @@
         <v>7.06</v>
       </c>
       <c r="N3" t="n">
-        <v>-4.51</v>
+        <v>-4.37</v>
       </c>
       <c r="O3" t="n">
         <v>0.49</v>
@@ -682,7 +682,7 @@
         <v>7.49</v>
       </c>
       <c r="N4" t="n">
-        <v>-9.369999999999999</v>
+        <v>-9.18</v>
       </c>
       <c r="O4" t="n">
         <v>-0.27</v>
@@ -742,7 +742,7 @@
         <v>26.64</v>
       </c>
       <c r="N5" t="n">
-        <v>-81.81</v>
+        <v>-80.67</v>
       </c>
       <c r="O5" t="n">
         <v>-0.31</v>
@@ -802,7 +802,7 @@
         <v>7.88</v>
       </c>
       <c r="N6" t="n">
-        <v>-8.84</v>
+        <v>-8.56</v>
       </c>
       <c r="O6" t="n">
         <v>-0.47</v>
@@ -862,7 +862,7 @@
         <v>5.85</v>
       </c>
       <c r="N7" t="n">
-        <v>-7.24</v>
+        <v>-7.37</v>
       </c>
       <c r="O7" t="n">
         <v>-0.68</v>
@@ -1019,7 +1019,7 @@
         <v>12.83</v>
       </c>
       <c r="N2" t="n">
-        <v>-5.88</v>
+        <v>-6.76</v>
       </c>
       <c r="O2" t="n">
         <v>0.58</v>
@@ -1079,7 +1079,7 @@
         <v>5.54</v>
       </c>
       <c r="N3" t="n">
-        <v>3.68</v>
+        <v>3.7</v>
       </c>
       <c r="O3" t="n">
         <v>-2.84</v>
@@ -1139,7 +1139,7 @@
         <v>15.8</v>
       </c>
       <c r="N4" t="n">
-        <v>-27.15</v>
+        <v>-26.12</v>
       </c>
       <c r="O4" t="n">
         <v>-0.11</v>
@@ -1199,7 +1199,7 @@
         <v>13.11</v>
       </c>
       <c r="N5" t="n">
-        <v>-16.35</v>
+        <v>-16.81</v>
       </c>
       <c r="O5" t="n">
         <v>-0.25</v>
@@ -1360,7 +1360,7 @@
         <v>11.12</v>
       </c>
       <c r="N2" t="n">
-        <v>-17.9</v>
+        <v>-17.47</v>
       </c>
       <c r="O2" t="n">
         <v>0.47</v>
@@ -1420,7 +1420,7 @@
         <v>8.640000000000001</v>
       </c>
       <c r="N3" t="n">
-        <v>-15.32</v>
+        <v>-16.01</v>
       </c>
       <c r="O3" t="n">
         <v>0.4</v>
@@ -1480,7 +1480,7 @@
         <v>10.84</v>
       </c>
       <c r="N4" t="n">
-        <v>-18.54</v>
+        <v>-17.69</v>
       </c>
       <c r="O4" t="n">
         <v>0.09</v>
@@ -1540,7 +1540,7 @@
         <v>7.52</v>
       </c>
       <c r="N5" t="n">
-        <v>-8.81</v>
+        <v>-8.949999999999999</v>
       </c>
       <c r="O5" t="n">
         <v>0.33</v>
@@ -1600,7 +1600,7 @@
         <v>17.11</v>
       </c>
       <c r="N6" t="n">
-        <v>-38.25</v>
+        <v>-37.91</v>
       </c>
       <c r="O6" t="n">
         <v>-0</v>
@@ -1660,7 +1660,7 @@
         <v>10.65</v>
       </c>
       <c r="N7" t="n">
-        <v>-16.35</v>
+        <v>-16.88</v>
       </c>
       <c r="O7" t="n">
         <v>0.23</v>
@@ -1720,7 +1720,7 @@
         <v>11.9</v>
       </c>
       <c r="N8" t="n">
-        <v>-18.73</v>
+        <v>-18.95</v>
       </c>
       <c r="O8" t="n">
         <v>-0.02</v>
@@ -1780,7 +1780,7 @@
         <v>16.13</v>
       </c>
       <c r="N9" t="n">
-        <v>-23.04</v>
+        <v>-23.22</v>
       </c>
       <c r="O9" t="n">
         <v>-0.45</v>
@@ -1840,7 +1840,7 @@
         <v>16.52</v>
       </c>
       <c r="N10" t="n">
-        <v>-35.3</v>
+        <v>-35.62</v>
       </c>
       <c r="O10" t="n">
         <v>0.08</v>
@@ -1900,7 +1900,7 @@
         <v>9.119999999999999</v>
       </c>
       <c r="N11" t="n">
-        <v>-1.52</v>
+        <v>-1.26</v>
       </c>
       <c r="O11" t="n">
         <v>0.83</v>

</xml_diff>

<commit_message>
add category optimization add constraints.py defining constraints for optimization
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -566,7 +566,7 @@
         <v>4.83</v>
       </c>
       <c r="N2" t="n">
-        <v>-10.43</v>
+        <v>-10.57</v>
       </c>
       <c r="O2" t="n">
         <v>0.37</v>
@@ -626,7 +626,7 @@
         <v>7.06</v>
       </c>
       <c r="N3" t="n">
-        <v>-4.37</v>
+        <v>-4.81</v>
       </c>
       <c r="O3" t="n">
         <v>0.49</v>
@@ -682,7 +682,7 @@
         <v>7.49</v>
       </c>
       <c r="N4" t="n">
-        <v>-9.18</v>
+        <v>-9.289999999999999</v>
       </c>
       <c r="O4" t="n">
         <v>-0.27</v>
@@ -742,7 +742,7 @@
         <v>26.64</v>
       </c>
       <c r="N5" t="n">
-        <v>-80.67</v>
+        <v>-82.09999999999999</v>
       </c>
       <c r="O5" t="n">
         <v>-0.31</v>
@@ -802,7 +802,7 @@
         <v>7.88</v>
       </c>
       <c r="N6" t="n">
-        <v>-8.56</v>
+        <v>-8.539999999999999</v>
       </c>
       <c r="O6" t="n">
         <v>-0.47</v>
@@ -862,7 +862,7 @@
         <v>5.85</v>
       </c>
       <c r="N7" t="n">
-        <v>-7.37</v>
+        <v>-7.38</v>
       </c>
       <c r="O7" t="n">
         <v>-0.68</v>
@@ -1019,7 +1019,7 @@
         <v>12.83</v>
       </c>
       <c r="N2" t="n">
-        <v>-6.76</v>
+        <v>-6.37</v>
       </c>
       <c r="O2" t="n">
         <v>0.58</v>
@@ -1079,7 +1079,7 @@
         <v>5.54</v>
       </c>
       <c r="N3" t="n">
-        <v>3.7</v>
+        <v>3.69</v>
       </c>
       <c r="O3" t="n">
         <v>-2.84</v>
@@ -1139,7 +1139,7 @@
         <v>15.8</v>
       </c>
       <c r="N4" t="n">
-        <v>-26.12</v>
+        <v>-26.16</v>
       </c>
       <c r="O4" t="n">
         <v>-0.11</v>
@@ -1199,7 +1199,7 @@
         <v>13.11</v>
       </c>
       <c r="N5" t="n">
-        <v>-16.81</v>
+        <v>-16.33</v>
       </c>
       <c r="O5" t="n">
         <v>-0.25</v>
@@ -1360,7 +1360,7 @@
         <v>11.12</v>
       </c>
       <c r="N2" t="n">
-        <v>-17.47</v>
+        <v>-17.55</v>
       </c>
       <c r="O2" t="n">
         <v>0.47</v>
@@ -1420,7 +1420,7 @@
         <v>8.640000000000001</v>
       </c>
       <c r="N3" t="n">
-        <v>-16.01</v>
+        <v>-15.7</v>
       </c>
       <c r="O3" t="n">
         <v>0.4</v>
@@ -1480,7 +1480,7 @@
         <v>10.84</v>
       </c>
       <c r="N4" t="n">
-        <v>-17.69</v>
+        <v>-18.5</v>
       </c>
       <c r="O4" t="n">
         <v>0.09</v>
@@ -1540,7 +1540,7 @@
         <v>7.52</v>
       </c>
       <c r="N5" t="n">
-        <v>-8.949999999999999</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="O5" t="n">
         <v>0.33</v>
@@ -1600,7 +1600,7 @@
         <v>17.11</v>
       </c>
       <c r="N6" t="n">
-        <v>-37.91</v>
+        <v>-37.84</v>
       </c>
       <c r="O6" t="n">
         <v>-0</v>
@@ -1660,7 +1660,7 @@
         <v>10.65</v>
       </c>
       <c r="N7" t="n">
-        <v>-16.88</v>
+        <v>-17.07</v>
       </c>
       <c r="O7" t="n">
         <v>0.23</v>
@@ -1720,7 +1720,7 @@
         <v>11.9</v>
       </c>
       <c r="N8" t="n">
-        <v>-18.95</v>
+        <v>-19.12</v>
       </c>
       <c r="O8" t="n">
         <v>-0.02</v>
@@ -1780,7 +1780,7 @@
         <v>16.13</v>
       </c>
       <c r="N9" t="n">
-        <v>-23.22</v>
+        <v>-23.39</v>
       </c>
       <c r="O9" t="n">
         <v>-0.45</v>
@@ -1840,7 +1840,7 @@
         <v>16.52</v>
       </c>
       <c r="N10" t="n">
-        <v>-35.62</v>
+        <v>-35.39</v>
       </c>
       <c r="O10" t="n">
         <v>0.08</v>
@@ -1900,7 +1900,7 @@
         <v>9.119999999999999</v>
       </c>
       <c r="N11" t="n">
-        <v>-1.26</v>
+        <v>-1.31</v>
       </c>
       <c r="O11" t="n">
         <v>0.83</v>

</xml_diff>

<commit_message>
add assign final asset weight for each security remove sub category risk weight
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -448,7 +448,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Sub Category Risk Weight</t>
+          <t>Sub Category Asset Weight</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Asset Weight</t>
+          <t>Portfolio Asset Weight</t>
         </is>
       </c>
     </row>
@@ -566,12 +566,14 @@
         <v>4.83</v>
       </c>
       <c r="N2" t="n">
-        <v>-10.57</v>
+        <v>-10.42</v>
       </c>
       <c r="O2" t="n">
         <v>0.37</v>
       </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>7.11</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -626,12 +628,14 @@
         <v>7.06</v>
       </c>
       <c r="N3" t="n">
-        <v>-4.81</v>
+        <v>-4.47</v>
       </c>
       <c r="O3" t="n">
         <v>0.49</v>
       </c>
-      <c r="P3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>12.89</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -682,12 +686,14 @@
         <v>7.49</v>
       </c>
       <c r="N4" t="n">
-        <v>-9.289999999999999</v>
+        <v>-9.18</v>
       </c>
       <c r="O4" t="n">
         <v>-0.27</v>
       </c>
-      <c r="P4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -742,12 +748,14 @@
         <v>26.64</v>
       </c>
       <c r="N5" t="n">
-        <v>-82.09999999999999</v>
+        <v>-80.28</v>
       </c>
       <c r="O5" t="n">
         <v>-0.31</v>
       </c>
-      <c r="P5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -802,12 +810,14 @@
         <v>7.88</v>
       </c>
       <c r="N6" t="n">
-        <v>-8.539999999999999</v>
+        <v>-8.720000000000001</v>
       </c>
       <c r="O6" t="n">
         <v>-0.47</v>
       </c>
-      <c r="P6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -862,12 +872,14 @@
         <v>5.85</v>
       </c>
       <c r="N7" t="n">
-        <v>-7.38</v>
+        <v>-7.56</v>
       </c>
       <c r="O7" t="n">
         <v>-0.68</v>
       </c>
-      <c r="P7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -901,7 +913,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Sub Category Risk Weight</t>
+          <t>Sub Category Asset Weight</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -966,7 +978,7 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Asset Weight</t>
+          <t>Portfolio Asset Weight</t>
         </is>
       </c>
     </row>
@@ -1019,12 +1031,14 @@
         <v>12.83</v>
       </c>
       <c r="N2" t="n">
-        <v>-6.37</v>
+        <v>-6.28</v>
       </c>
       <c r="O2" t="n">
         <v>0.58</v>
       </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>28.12</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1079,12 +1093,14 @@
         <v>5.54</v>
       </c>
       <c r="N3" t="n">
-        <v>3.69</v>
+        <v>3.68</v>
       </c>
       <c r="O3" t="n">
         <v>-2.84</v>
       </c>
-      <c r="P3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>4.69</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1139,12 +1155,14 @@
         <v>15.8</v>
       </c>
       <c r="N4" t="n">
-        <v>-26.16</v>
+        <v>-26.39</v>
       </c>
       <c r="O4" t="n">
         <v>-0.11</v>
       </c>
-      <c r="P4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>4.69</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1199,12 +1217,14 @@
         <v>13.11</v>
       </c>
       <c r="N5" t="n">
-        <v>-16.33</v>
+        <v>-16.85</v>
       </c>
       <c r="O5" t="n">
         <v>-0.25</v>
       </c>
-      <c r="P5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>12.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1217,7 +1237,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1238,7 +1258,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Sub Category Risk Weight</t>
+          <t>Sub Category Asset Weight</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -1303,7 +1323,7 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Asset Weight</t>
+          <t>Portfolio Asset Weight</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1339,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>19.8</v>
+        <v>29.6</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1360,12 +1380,14 @@
         <v>11.12</v>
       </c>
       <c r="N2" t="n">
-        <v>-17.55</v>
+        <v>-18.35</v>
       </c>
       <c r="O2" t="n">
         <v>0.47</v>
       </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>5.33</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1379,7 +1401,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4.95</v>
+        <v>12.95</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1420,17 +1442,19 @@
         <v>8.640000000000001</v>
       </c>
       <c r="N3" t="n">
-        <v>-15.7</v>
+        <v>-15.37</v>
       </c>
       <c r="O3" t="n">
         <v>0.4</v>
       </c>
-      <c r="P3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>2.33</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLJP</t>
+          <t>FLJH</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1439,11 +1463,11 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9.9</v>
+        <v>17.9</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Franklin FTSE Japan ETF</t>
+          <t>Franklin FTSE Japan Hedged ETF</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1465,27 +1489,29 @@
         <v>0.09</v>
       </c>
       <c r="I4" t="n">
-        <v>2.24</v>
+        <v>0.88</v>
       </c>
       <c r="J4" t="n">
-        <v>4.22</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>6.48</v>
+        <v>10.1</v>
       </c>
       <c r="L4" t="n">
-        <v>14.83</v>
+        <v>21.4</v>
       </c>
       <c r="M4" t="n">
-        <v>10.84</v>
+        <v>12.49</v>
       </c>
       <c r="N4" t="n">
-        <v>-18.5</v>
+        <v>-24.76</v>
       </c>
       <c r="O4" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="P4" t="inlineStr"/>
+        <v>0.23</v>
+      </c>
+      <c r="P4" t="n">
+        <v>3.22</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1499,7 +1525,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7.43</v>
+        <v>15.43</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1540,17 +1566,19 @@
         <v>7.52</v>
       </c>
       <c r="N5" t="n">
-        <v>-8.890000000000001</v>
+        <v>-8.380000000000001</v>
       </c>
       <c r="O5" t="n">
         <v>0.33</v>
       </c>
-      <c r="P5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>2.78</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FLKR</t>
+          <t>EWX</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1559,16 +1587,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7.43</v>
+        <v>24.12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Franklin FTSE South Korea ETF</t>
+          <t>SPDR S&amp;P Emerging Markets Small Cap ETF</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Diversified Emerging Mkts</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1582,53 +1610,55 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0.09</v>
+        <v>0.65</v>
       </c>
       <c r="I6" t="n">
-        <v>3.75</v>
+        <v>2.54</v>
       </c>
       <c r="J6" t="n">
-        <v>1.3</v>
+        <v>6.52</v>
       </c>
       <c r="K6" t="n">
-        <v>5.15</v>
+        <v>9.08</v>
       </c>
       <c r="L6" t="n">
-        <v>26.45</v>
+        <v>13.91</v>
       </c>
       <c r="M6" t="n">
-        <v>17.11</v>
+        <v>10.13</v>
       </c>
       <c r="N6" t="n">
-        <v>-37.84</v>
+        <v>-14.14</v>
       </c>
       <c r="O6" t="n">
-        <v>-0</v>
-      </c>
-      <c r="P6" t="inlineStr"/>
+        <v>0.28</v>
+      </c>
+      <c r="P6" t="n">
+        <v>4.34</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SPEU</t>
+          <t>VNQ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Traditional Equity</t>
+          <t>REIT</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>24.75</v>
+        <v>100</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SPDR Portfolio Europe ETF</t>
+          <t>Vanguard Real Estate Index Fund</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Europe Stock</t>
+          <t>Real Estate</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1642,58 +1672,60 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="I7" t="n">
-        <v>3.33</v>
+        <v>4.92</v>
       </c>
       <c r="J7" t="n">
-        <v>5.31</v>
+        <v>2.35</v>
       </c>
       <c r="K7" t="n">
-        <v>8.67</v>
+        <v>7.4</v>
       </c>
       <c r="L7" t="n">
-        <v>15.35</v>
+        <v>26.07</v>
       </c>
       <c r="M7" t="n">
-        <v>10.65</v>
+        <v>16.52</v>
       </c>
       <c r="N7" t="n">
-        <v>-17.07</v>
+        <v>-35.24</v>
       </c>
       <c r="O7" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="P7" t="inlineStr"/>
+        <v>0.08</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SPEM</t>
+          <t>PDBC</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Traditional Equity</t>
+          <t>Commodity</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>25.74</v>
+        <v>100</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SPDR Portfolio Emerging Markets ETF</t>
+          <t>Invesco Optimum Yield Diversified Commodity Strategy No K-1 ETF</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Diversified Emerging Mkts</t>
+          <t>Commodities Broad Basket</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>NasdaqGM</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1702,210 +1734,32 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.59</v>
       </c>
       <c r="I8" t="n">
-        <v>3.39</v>
+        <v>12.91</v>
       </c>
       <c r="J8" t="n">
-        <v>1.58</v>
+        <v>-1.11</v>
       </c>
       <c r="K8" t="n">
-        <v>5</v>
+        <v>11.83</v>
       </c>
       <c r="L8" t="n">
-        <v>14.48</v>
+        <v>7.96</v>
       </c>
       <c r="M8" t="n">
-        <v>11.9</v>
+        <v>9.119999999999999</v>
       </c>
       <c r="N8" t="n">
-        <v>-19.12</v>
+        <v>-0.58</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.02</v>
-      </c>
-      <c r="P8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>RWX</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>REIT</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>50</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>SPDR Dow Jones International Real Estate ETF</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Global Real Estate</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="I9" t="n">
-        <v>5.41</v>
-      </c>
-      <c r="J9" t="n">
-        <v>-6.33</v>
-      </c>
-      <c r="K9" t="n">
-        <v>-0.88</v>
-      </c>
-      <c r="L9" t="n">
-        <v>13.66</v>
-      </c>
-      <c r="M9" t="n">
-        <v>16.13</v>
-      </c>
-      <c r="N9" t="n">
-        <v>-23.39</v>
-      </c>
-      <c r="O9" t="n">
-        <v>-0.45</v>
-      </c>
-      <c r="P9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>VNQ</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>REIT</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>50</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Vanguard Real Estate Index Fund</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Real Estate</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>NYSEArca</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="I10" t="n">
-        <v>4.92</v>
-      </c>
-      <c r="J10" t="n">
-        <v>2.35</v>
-      </c>
-      <c r="K10" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="L10" t="n">
-        <v>26.07</v>
-      </c>
-      <c r="M10" t="n">
-        <v>16.52</v>
-      </c>
-      <c r="N10" t="n">
-        <v>-35.39</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="P10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>PDBC</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Commodity</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>100</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Invesco Optimum Yield Diversified Commodity Strategy No K-1 ETF</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Commodities Broad Basket</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>NasdaqGM</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="I11" t="n">
-        <v>12.91</v>
-      </c>
-      <c r="J11" t="n">
-        <v>-1.11</v>
-      </c>
-      <c r="K11" t="n">
-        <v>11.83</v>
-      </c>
-      <c r="L11" t="n">
-        <v>7.96</v>
-      </c>
-      <c r="M11" t="n">
-        <v>9.119999999999999</v>
-      </c>
-      <c r="N11" t="n">
-        <v>-1.31</v>
-      </c>
-      <c r="O11" t="n">
         <v>0.83</v>
       </c>
-      <c r="P11" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix fetch_dividend_yield add avg_dividend_yield from dividends history
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,40 +483,45 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Average Dividend Yield</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Simple Return</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Total Return</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Standard Deviation</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Downside Deviation</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Value at Risk 95%</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Sharpe Ratio</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Portfolio Asset Weight</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Portfolio Asset Allocation</t>
         </is>
@@ -534,7 +539,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -559,54 +564,53 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>9.300000000000001</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>9.300000000000001</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="L2" t="n">
-        <v>12.52</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>3.21</v>
+        <v>12.18</v>
       </c>
       <c r="N2" t="n">
-        <v>-11.34</v>
+        <v>2.89</v>
       </c>
       <c r="O2" t="n">
-        <v>0.58</v>
+        <v>-10.84</v>
       </c>
       <c r="P2" t="n">
-        <v>6.61</v>
+        <v>0.59</v>
       </c>
       <c r="Q2" t="n">
-        <v>660.5599999999999</v>
+        <v>1.6</v>
+      </c>
+      <c r="R2" t="n">
+        <v>160.3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DBMF</t>
+          <t>PPLT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Managed Futures</t>
+          <t>Metal</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>iMGP DBi Managed Futures Strategy ETF</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Managed Futures</t>
-        </is>
-      </c>
+          <t>abrdn Physical Platinum Shares ETF</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
           <t>NYSEArca</t>
@@ -618,45 +622,48 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.85</v>
+        <v>0.6</v>
       </c>
       <c r="I3" t="n">
-        <v>7.81</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>1.53</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>9.359999999999999</v>
+        <v>2.94</v>
       </c>
       <c r="L3" t="n">
-        <v>8.01</v>
+        <v>2.94</v>
       </c>
       <c r="M3" t="n">
-        <v>4.53</v>
+        <v>14.84</v>
       </c>
       <c r="N3" t="n">
-        <v>-3.88</v>
+        <v>8.75</v>
       </c>
       <c r="O3" t="n">
-        <v>0.92</v>
+        <v>-21.22</v>
       </c>
       <c r="P3" t="n">
-        <v>13.39</v>
+        <v>0.06</v>
       </c>
       <c r="Q3" t="n">
-        <v>1339.44</v>
+        <v>1.6</v>
+      </c>
+      <c r="R3" t="n">
+        <v>160.3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>QAI</t>
+          <t>DBMF</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Global Macro</t>
+          <t>Managed Futures</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -664,10 +671,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>IQ Hedge Multi-Strategy Tracker ETF</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>iMGP DBi Managed Futures Strategy ETF</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Managed Futures</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>NYSEArca</t>
@@ -679,45 +690,48 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0.78</v>
+        <v>0.85</v>
       </c>
       <c r="I4" t="n">
-        <v>1.91</v>
+        <v>8.23</v>
       </c>
       <c r="J4" t="n">
-        <v>1.2</v>
+        <v>7.06</v>
       </c>
       <c r="K4" t="n">
-        <v>3.11</v>
+        <v>1.27</v>
       </c>
       <c r="L4" t="n">
-        <v>7.38</v>
+        <v>9.52</v>
       </c>
       <c r="M4" t="n">
-        <v>5.67</v>
+        <v>8.73</v>
       </c>
       <c r="N4" t="n">
-        <v>-8.779999999999999</v>
+        <v>5.29</v>
       </c>
       <c r="O4" t="n">
-        <v>0.15</v>
+        <v>-4.76</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>7.48</v>
+      </c>
+      <c r="R4" t="n">
+        <v>748.09</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VIXM</t>
+          <t>QAI</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VIX Futures</t>
+          <t>Global Macro</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -725,17 +739,13 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ProShares VIX Mid-Term Futures ETF</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Trading--Miscellaneous</t>
-        </is>
-      </c>
+          <t>IQ Hedge Multi-Strategy Tracker ETF</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Cboe US</t>
+          <t>NYSEArca</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -744,63 +754,66 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0.93</v>
+        <v>0.78</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1.86</v>
       </c>
       <c r="J5" t="n">
-        <v>-8.06</v>
+        <v>1.61</v>
       </c>
       <c r="K5" t="n">
-        <v>-8.06</v>
+        <v>1.44</v>
       </c>
       <c r="L5" t="n">
-        <v>45.53</v>
+        <v>3.3</v>
       </c>
       <c r="M5" t="n">
-        <v>23.98</v>
+        <v>7.66</v>
       </c>
       <c r="N5" t="n">
-        <v>-82.83</v>
+        <v>5.68</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.22</v>
+        <v>-8.99</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="Q5" t="n">
         <v>0</v>
       </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FXB</t>
+          <t>VIXM</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Currency</t>
+          <t>VIX Futures</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Invesco CurrencyShares British Pound Sterling Trust</t>
+          <t>ProShares VIX Mid-Term Futures ETF</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Single Currency</t>
+          <t>Trading--Miscellaneous</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>NYSEArca</t>
+          <t>Cboe US</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -809,40 +822,43 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0.4</v>
+        <v>0.93</v>
       </c>
       <c r="I6" t="n">
-        <v>2.38</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>2.08</v>
+        <v>-9.25</v>
       </c>
       <c r="L6" t="n">
-        <v>6.57</v>
+        <v>-9.25</v>
       </c>
       <c r="M6" t="n">
-        <v>6.03</v>
+        <v>44.7</v>
       </c>
       <c r="N6" t="n">
-        <v>-8.640000000000001</v>
+        <v>25.02</v>
       </c>
       <c r="O6" t="n">
-        <v>0.01</v>
+        <v>-83.45</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
       </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FXF</t>
+          <t>FXB</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -855,7 +871,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Invesco CurrencyShares Swiss Franc Trust</t>
+          <t>Invesco CurrencyShares British Pound Sterling Trust</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -877,30 +893,101 @@
         <v>0.4</v>
       </c>
       <c r="I7" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-0.28</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="M7" t="n">
+        <v>6.51</v>
+      </c>
+      <c r="N7" t="n">
+        <v>5.96</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-8.32</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Q7" t="n">
         <v>0</v>
       </c>
-      <c r="J7" t="n">
-        <v>1.49</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1.49</v>
-      </c>
-      <c r="L7" t="n">
-        <v>5.51</v>
-      </c>
-      <c r="M7" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="N7" t="n">
-        <v>-7.58</v>
-      </c>
-      <c r="O7" t="n">
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>FXF</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>50</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Invesco CurrencyShares Swiss Franc Trust</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Single Currency</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="M8" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="N8" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-7.74</v>
+      </c>
+      <c r="P8" t="n">
         <v>-0.09</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q8" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -915,7 +1002,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -971,40 +1058,45 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Average Dividend Yield</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Simple Return</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Total Return</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Standard Deviation</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Downside Deviation</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Value at Risk 95%</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Sharpe Ratio</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Portfolio Asset Weight</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Portfolio Asset Allocation</t>
         </is>
@@ -1044,31 +1136,34 @@
         <v>0.25</v>
       </c>
       <c r="I2" t="n">
-        <v>15.17</v>
+        <v>14.21</v>
       </c>
       <c r="J2" t="n">
-        <v>-3.74</v>
+        <v>4.77</v>
       </c>
       <c r="K2" t="n">
-        <v>11.51</v>
+        <v>-3.52</v>
       </c>
       <c r="L2" t="n">
-        <v>10.69</v>
+        <v>10.77</v>
       </c>
       <c r="M2" t="n">
-        <v>10.8</v>
+        <v>11.02</v>
       </c>
       <c r="N2" t="n">
-        <v>-5.85</v>
+        <v>10.88</v>
       </c>
       <c r="O2" t="n">
-        <v>0.89</v>
+        <v>-7.5</v>
       </c>
       <c r="P2" t="n">
-        <v>28.12</v>
+        <v>0.8</v>
       </c>
       <c r="Q2" t="n">
-        <v>2812.5</v>
+        <v>32.1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>3210.21</v>
       </c>
     </row>
     <row r="3">
@@ -1109,31 +1204,34 @@
         <v>0.135</v>
       </c>
       <c r="I3" t="n">
-        <v>4.57</v>
+        <v>4.73</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.32</v>
+        <v>3.07</v>
       </c>
       <c r="K3" t="n">
-        <v>4.25</v>
+        <v>-0.25</v>
       </c>
       <c r="L3" t="n">
-        <v>0.34</v>
+        <v>4.48</v>
       </c>
       <c r="M3" t="n">
-        <v>2.34</v>
+        <v>0.4</v>
       </c>
       <c r="N3" t="n">
-        <v>3.68</v>
+        <v>2.27</v>
       </c>
       <c r="O3" t="n">
-        <v>6.6</v>
+        <v>3.81</v>
       </c>
       <c r="P3" t="n">
-        <v>4.69</v>
+        <v>6.15</v>
       </c>
       <c r="Q3" t="n">
-        <v>469</v>
+        <v>5.35</v>
+      </c>
+      <c r="R3" t="n">
+        <v>535.3200000000001</v>
       </c>
     </row>
     <row r="4">
@@ -1171,34 +1269,37 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="I4" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-1.11</v>
+      </c>
+      <c r="L4" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="M4" t="n">
+        <v>18.18</v>
+      </c>
+      <c r="N4" t="n">
+        <v>13.93</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-26.2</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Q4" t="n">
         <v>5.35</v>
       </c>
-      <c r="J4" t="n">
-        <v>-2.33</v>
-      </c>
-      <c r="K4" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="L4" t="n">
-        <v>17.6</v>
-      </c>
-      <c r="M4" t="n">
-        <v>13.76</v>
-      </c>
-      <c r="N4" t="n">
-        <v>-25.12</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="P4" t="n">
-        <v>4.69</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>469</v>
+      <c r="R4" t="n">
+        <v>535.3200000000001</v>
       </c>
     </row>
     <row r="5">
@@ -1239,31 +1340,102 @@
         <v>0.2</v>
       </c>
       <c r="I5" t="n">
-        <v>5.97</v>
+        <v>5.67</v>
       </c>
       <c r="J5" t="n">
-        <v>-3.82</v>
+        <v>3.92</v>
       </c>
       <c r="K5" t="n">
-        <v>2.19</v>
+        <v>-3.07</v>
       </c>
       <c r="L5" t="n">
-        <v>11.32</v>
+        <v>2.63</v>
       </c>
       <c r="M5" t="n">
-        <v>10.94</v>
+        <v>11.93</v>
       </c>
       <c r="N5" t="n">
-        <v>-16.13</v>
+        <v>11.04</v>
       </c>
       <c r="O5" t="n">
-        <v>0.02</v>
+        <v>-17.08</v>
       </c>
       <c r="P5" t="n">
-        <v>12.5</v>
+        <v>0.05</v>
       </c>
       <c r="Q5" t="n">
-        <v>1250</v>
+        <v>14.27</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1426.76</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PAVE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Infrastructure</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Global X U.S. Infrastructure Development ETF</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Infrastructure</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Cboe US</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="K6" t="n">
+        <v>20.36</v>
+      </c>
+      <c r="L6" t="n">
+        <v>21.07</v>
+      </c>
+      <c r="M6" t="n">
+        <v>17.62</v>
+      </c>
+      <c r="N6" t="n">
+        <v>4.47</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-8.42</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="R6" t="n">
+        <v>224.26</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1333,40 +1505,45 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Average Dividend Yield</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Simple Return</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Total Return</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Standard Deviation</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Downside Deviation</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Value at Risk 95%</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Sharpe Ratio</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Portfolio Asset Weight</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Portfolio Asset Allocation</t>
         </is>
@@ -1384,7 +1561,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>29.6</v>
+        <v>26.64</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1407,34 +1584,37 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I2" t="n">
-        <v>1.62</v>
+        <v>1.48</v>
       </c>
       <c r="J2" t="n">
-        <v>12.68</v>
+        <v>1.33</v>
       </c>
       <c r="K2" t="n">
-        <v>14.32</v>
+        <v>13.51</v>
       </c>
       <c r="L2" t="n">
-        <v>19.95</v>
+        <v>15.02</v>
       </c>
       <c r="M2" t="n">
-        <v>9.779999999999999</v>
+        <v>20.03</v>
       </c>
       <c r="N2" t="n">
-        <v>-18.53</v>
+        <v>9.68</v>
       </c>
       <c r="O2" t="n">
-        <v>0.62</v>
+        <v>-17.33</v>
       </c>
       <c r="P2" t="n">
-        <v>5.33</v>
+        <v>0.65</v>
       </c>
       <c r="Q2" t="n">
-        <v>532.8</v>
+        <v>4.8</v>
+      </c>
+      <c r="R2" t="n">
+        <v>479.52</v>
       </c>
     </row>
     <row r="3">
@@ -1449,7 +1629,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12.95</v>
+        <v>11.66</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1475,31 +1655,34 @@
         <v>0.09</v>
       </c>
       <c r="I3" t="n">
-        <v>3.17</v>
+        <v>2.87</v>
       </c>
       <c r="J3" t="n">
-        <v>8.539999999999999</v>
+        <v>2.02</v>
       </c>
       <c r="K3" t="n">
-        <v>11.74</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>16.86</v>
+        <v>11.68</v>
       </c>
       <c r="M3" t="n">
-        <v>7.29</v>
+        <v>16.71</v>
       </c>
       <c r="N3" t="n">
-        <v>-15.77</v>
+        <v>7.17</v>
       </c>
       <c r="O3" t="n">
+        <v>-15.19</v>
+      </c>
+      <c r="P3" t="n">
         <v>0.58</v>
       </c>
-      <c r="P3" t="n">
-        <v>2.33</v>
-      </c>
       <c r="Q3" t="n">
-        <v>233.1</v>
+        <v>2.1</v>
+      </c>
+      <c r="R3" t="n">
+        <v>209.88</v>
       </c>
     </row>
     <row r="4">
@@ -1514,7 +1697,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17.9</v>
+        <v>16.11</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1540,37 +1723,40 @@
         <v>0.09</v>
       </c>
       <c r="I4" t="n">
-        <v>0.88</v>
+        <v>0.83</v>
       </c>
       <c r="J4" t="n">
-        <v>8.890000000000001</v>
+        <v>8.77</v>
       </c>
       <c r="K4" t="n">
-        <v>9.789999999999999</v>
+        <v>3.76</v>
       </c>
       <c r="L4" t="n">
-        <v>20.95</v>
+        <v>4.6</v>
       </c>
       <c r="M4" t="n">
-        <v>11.06</v>
+        <v>16.38</v>
       </c>
       <c r="N4" t="n">
-        <v>-24.96</v>
+        <v>11.05</v>
       </c>
       <c r="O4" t="n">
-        <v>0.37</v>
+        <v>-22.35</v>
       </c>
       <c r="P4" t="n">
-        <v>3.22</v>
+        <v>0.16</v>
       </c>
       <c r="Q4" t="n">
-        <v>322.2</v>
+        <v>2.9</v>
+      </c>
+      <c r="R4" t="n">
+        <v>289.98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLAU</t>
+          <t>SPEU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1579,16 +1765,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>15.43</v>
+        <v>10</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Franklin FTSE Australia ETF</t>
+          <t>SPDR Portfolio Europe ETF</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Miscellaneous Region</t>
+          <t>Europe Stock</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1602,40 +1788,43 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I5" t="n">
-        <v>4.72</v>
+        <v>3.03</v>
       </c>
       <c r="J5" t="n">
-        <v>3.81</v>
+        <v>2.39</v>
       </c>
       <c r="K5" t="n">
-        <v>8.550000000000001</v>
+        <v>5.77</v>
       </c>
       <c r="L5" t="n">
-        <v>11.03</v>
+        <v>8.83</v>
       </c>
       <c r="M5" t="n">
-        <v>6.19</v>
+        <v>15.6</v>
       </c>
       <c r="N5" t="n">
-        <v>-9.57</v>
+        <v>9.18</v>
       </c>
       <c r="O5" t="n">
-        <v>0.59</v>
+        <v>-17.11</v>
       </c>
       <c r="P5" t="n">
-        <v>2.78</v>
+        <v>0.44</v>
       </c>
       <c r="Q5" t="n">
-        <v>277.74</v>
+        <v>1.8</v>
+      </c>
+      <c r="R5" t="n">
+        <v>180</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EWX</t>
+          <t>FLAU</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1644,16 +1833,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>24.12</v>
+        <v>13.89</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SPDR S&amp;P Emerging Markets Small Cap ETF</t>
+          <t>Franklin FTSE Australia ETF</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Diversified Emerging Mkts</t>
+          <t>Miscellaneous Region</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1667,58 +1856,61 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0.65</v>
+        <v>0.09</v>
       </c>
       <c r="I6" t="n">
-        <v>2.54</v>
+        <v>4.3</v>
       </c>
       <c r="J6" t="n">
-        <v>6.32</v>
+        <v>3.6</v>
       </c>
       <c r="K6" t="n">
-        <v>8.880000000000001</v>
+        <v>4.36</v>
       </c>
       <c r="L6" t="n">
-        <v>13.79</v>
+        <v>8.68</v>
       </c>
       <c r="M6" t="n">
-        <v>8.68</v>
+        <v>10.6</v>
       </c>
       <c r="N6" t="n">
-        <v>-14.55</v>
+        <v>6</v>
       </c>
       <c r="O6" t="n">
-        <v>0.5</v>
+        <v>-8.6</v>
       </c>
       <c r="P6" t="n">
-        <v>4.34</v>
+        <v>0.63</v>
       </c>
       <c r="Q6" t="n">
-        <v>434.16</v>
+        <v>2.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>250.02</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>VNQ</t>
+          <t>EWX</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>REIT</t>
+          <t>Traditional Equity</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>100</v>
+        <v>21.71</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Vanguard Real Estate Index Fund</t>
+          <t>SPDR S&amp;P Emerging Markets Small Cap ETF</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Real Estate</t>
+          <t>Diversified Emerging Mkts</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1732,34 +1924,37 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>0.1</v>
+        <v>0.65</v>
       </c>
       <c r="I7" t="n">
-        <v>4.92</v>
+        <v>2.36</v>
       </c>
       <c r="J7" t="n">
-        <v>2.57</v>
+        <v>2.29</v>
       </c>
       <c r="K7" t="n">
-        <v>7.62</v>
+        <v>6.6</v>
       </c>
       <c r="L7" t="n">
-        <v>26.28</v>
+        <v>8.98</v>
       </c>
       <c r="M7" t="n">
-        <v>14.53</v>
+        <v>13.97</v>
       </c>
       <c r="N7" t="n">
-        <v>-35.32</v>
+        <v>8.69</v>
       </c>
       <c r="O7" t="n">
-        <v>0.21</v>
+        <v>-14.04</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>3.91</v>
+      </c>
+      <c r="R7" t="n">
+        <v>390.78</v>
       </c>
     </row>
     <row r="8">
@@ -1803,28 +1998,95 @@
         <v>12.91</v>
       </c>
       <c r="J8" t="n">
-        <v>-1.21</v>
+        <v>13.26</v>
       </c>
       <c r="K8" t="n">
-        <v>11.73</v>
+        <v>-1.55</v>
       </c>
       <c r="L8" t="n">
-        <v>7.86</v>
+        <v>11.39</v>
       </c>
       <c r="M8" t="n">
-        <v>6.68</v>
+        <v>8.18</v>
       </c>
       <c r="N8" t="n">
-        <v>-1.34</v>
+        <v>7.08</v>
       </c>
       <c r="O8" t="n">
-        <v>1.24</v>
+        <v>-2.26</v>
       </c>
       <c r="P8" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="Q8" t="n">
         <v>12</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>1200</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DBO</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>100</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Invesco DB Oil Fund</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>NYSEArca</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="K9" t="n">
+        <v>11.91</v>
+      </c>
+      <c r="L9" t="n">
+        <v>12.57</v>
+      </c>
+      <c r="M9" t="n">
+        <v>30.85</v>
+      </c>
+      <c r="N9" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-38.13</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add DIVIDEND_TYPE in global_settings.py
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -579,16 +579,16 @@
         <v>2.89</v>
       </c>
       <c r="O2" t="n">
-        <v>-10.84</v>
+        <v>-10.6</v>
       </c>
       <c r="P2" t="n">
         <v>0.59</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.6</v>
+        <v>4.5</v>
       </c>
       <c r="R2" t="n">
-        <v>160.3</v>
+        <v>450</v>
       </c>
     </row>
     <row r="3">
@@ -643,16 +643,16 @@
         <v>8.75</v>
       </c>
       <c r="O3" t="n">
-        <v>-21.22</v>
+        <v>-21.69</v>
       </c>
       <c r="P3" t="n">
         <v>0.06</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.6</v>
+        <v>4.5</v>
       </c>
       <c r="R3" t="n">
-        <v>160.3</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4">
@@ -711,16 +711,16 @@
         <v>5.29</v>
       </c>
       <c r="O4" t="n">
-        <v>-4.76</v>
+        <v>-5.18</v>
       </c>
       <c r="P4" t="n">
         <v>0.86</v>
       </c>
       <c r="Q4" t="n">
-        <v>7.48</v>
+        <v>21</v>
       </c>
       <c r="R4" t="n">
-        <v>748.09</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="5">
@@ -775,7 +775,7 @@
         <v>5.68</v>
       </c>
       <c r="O5" t="n">
-        <v>-8.99</v>
+        <v>-9.220000000000001</v>
       </c>
       <c r="P5" t="n">
         <v>0.17</v>
@@ -843,7 +843,7 @@
         <v>25.02</v>
       </c>
       <c r="O6" t="n">
-        <v>-83.45</v>
+        <v>-82.92</v>
       </c>
       <c r="P6" t="n">
         <v>-0.25</v>
@@ -911,7 +911,7 @@
         <v>5.96</v>
       </c>
       <c r="O7" t="n">
-        <v>-8.32</v>
+        <v>-8.5</v>
       </c>
       <c r="P7" t="n">
         <v>0.03</v>
@@ -979,7 +979,7 @@
         <v>3.49</v>
       </c>
       <c r="O8" t="n">
-        <v>-7.74</v>
+        <v>-7.19</v>
       </c>
       <c r="P8" t="n">
         <v>-0.09</v>
@@ -1154,16 +1154,16 @@
         <v>10.88</v>
       </c>
       <c r="O2" t="n">
-        <v>-7.5</v>
+        <v>-7.64</v>
       </c>
       <c r="P2" t="n">
         <v>0.8</v>
       </c>
       <c r="Q2" t="n">
-        <v>32.1</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>3210.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1222,16 +1222,16 @@
         <v>2.27</v>
       </c>
       <c r="O3" t="n">
-        <v>3.81</v>
+        <v>3.82</v>
       </c>
       <c r="P3" t="n">
         <v>6.15</v>
       </c>
       <c r="Q3" t="n">
-        <v>5.35</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>535.3200000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1290,16 +1290,16 @@
         <v>13.93</v>
       </c>
       <c r="O4" t="n">
-        <v>-26.2</v>
+        <v>-26.47</v>
       </c>
       <c r="P4" t="n">
         <v>0.1</v>
       </c>
       <c r="Q4" t="n">
-        <v>5.35</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>535.3200000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1358,16 +1358,16 @@
         <v>11.04</v>
       </c>
       <c r="O5" t="n">
-        <v>-17.08</v>
+        <v>-16.96</v>
       </c>
       <c r="P5" t="n">
         <v>0.05</v>
       </c>
       <c r="Q5" t="n">
-        <v>14.27</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>1426.76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1426,16 +1426,16 @@
         <v>4.47</v>
       </c>
       <c r="O6" t="n">
-        <v>-8.42</v>
+        <v>-7.04</v>
       </c>
       <c r="P6" t="n">
         <v>1.08</v>
       </c>
       <c r="Q6" t="n">
-        <v>2.24</v>
+        <v>12.22</v>
       </c>
       <c r="R6" t="n">
-        <v>224.26</v>
+        <v>1221.6</v>
       </c>
     </row>
   </sheetData>
@@ -1605,16 +1605,16 @@
         <v>9.68</v>
       </c>
       <c r="O2" t="n">
-        <v>-17.33</v>
+        <v>-17.75</v>
       </c>
       <c r="P2" t="n">
         <v>0.65</v>
       </c>
       <c r="Q2" t="n">
-        <v>4.8</v>
+        <v>9.24</v>
       </c>
       <c r="R2" t="n">
-        <v>479.52</v>
+        <v>923.62</v>
       </c>
     </row>
     <row r="3">
@@ -1673,16 +1673,16 @@
         <v>7.17</v>
       </c>
       <c r="O3" t="n">
-        <v>-15.19</v>
+        <v>-15.72</v>
       </c>
       <c r="P3" t="n">
         <v>0.58</v>
       </c>
       <c r="Q3" t="n">
-        <v>2.1</v>
+        <v>4.04</v>
       </c>
       <c r="R3" t="n">
-        <v>209.88</v>
+        <v>404.26</v>
       </c>
     </row>
     <row r="4">
@@ -1741,16 +1741,16 @@
         <v>11.05</v>
       </c>
       <c r="O4" t="n">
-        <v>-22.35</v>
+        <v>-22.17</v>
       </c>
       <c r="P4" t="n">
         <v>0.16</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.9</v>
+        <v>5.59</v>
       </c>
       <c r="R4" t="n">
-        <v>289.98</v>
+        <v>558.54</v>
       </c>
     </row>
     <row r="5">
@@ -1809,16 +1809,16 @@
         <v>9.18</v>
       </c>
       <c r="O5" t="n">
-        <v>-17.11</v>
+        <v>-16.75</v>
       </c>
       <c r="P5" t="n">
         <v>0.44</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.8</v>
+        <v>3.47</v>
       </c>
       <c r="R5" t="n">
-        <v>180</v>
+        <v>346.7</v>
       </c>
     </row>
     <row r="6">
@@ -1877,16 +1877,16 @@
         <v>6</v>
       </c>
       <c r="O6" t="n">
-        <v>-8.6</v>
+        <v>-8.359999999999999</v>
       </c>
       <c r="P6" t="n">
         <v>0.63</v>
       </c>
       <c r="Q6" t="n">
-        <v>2.5</v>
+        <v>4.82</v>
       </c>
       <c r="R6" t="n">
-        <v>250.02</v>
+        <v>481.57</v>
       </c>
     </row>
     <row r="7">
@@ -1945,16 +1945,16 @@
         <v>8.69</v>
       </c>
       <c r="O7" t="n">
-        <v>-14.04</v>
+        <v>-14.01</v>
       </c>
       <c r="P7" t="n">
         <v>0.5</v>
       </c>
       <c r="Q7" t="n">
-        <v>3.91</v>
+        <v>7.53</v>
       </c>
       <c r="R7" t="n">
-        <v>390.78</v>
+        <v>752.6900000000001</v>
       </c>
     </row>
     <row r="8">
@@ -2013,16 +2013,16 @@
         <v>7.08</v>
       </c>
       <c r="O8" t="n">
-        <v>-2.26</v>
+        <v>-1.79</v>
       </c>
       <c r="P8" t="n">
         <v>1.15</v>
       </c>
       <c r="Q8" t="n">
-        <v>12</v>
+        <v>23.11</v>
       </c>
       <c r="R8" t="n">
-        <v>1200</v>
+        <v>2311.36</v>
       </c>
     </row>
     <row r="9">
@@ -2077,7 +2077,7 @@
         <v>10.44</v>
       </c>
       <c r="O9" t="n">
-        <v>-38.13</v>
+        <v>-37.5</v>
       </c>
       <c r="P9" t="n">
         <v>0.34</v>

</xml_diff>

<commit_message>
add number_of_shares in security.py and excel_writer.py
</commit_message>
<xml_diff>
--- a/src/ETF.xlsx
+++ b/src/ETF.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +526,11 @@
           <t>Portfolio Asset Allocation</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Shares</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -567,22 +572,22 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>9.210000000000001</v>
+        <v>9.31</v>
       </c>
       <c r="L2" t="n">
-        <v>9.210000000000001</v>
+        <v>9.31</v>
       </c>
       <c r="M2" t="n">
-        <v>12.18</v>
+        <v>12.19</v>
       </c>
       <c r="N2" t="n">
         <v>2.89</v>
       </c>
       <c r="O2" t="n">
-        <v>-10.6</v>
+        <v>-10.61</v>
       </c>
       <c r="P2" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="Q2" t="n">
         <v>4.5</v>
@@ -590,6 +595,9 @@
       <c r="R2" t="n">
         <v>450</v>
       </c>
+      <c r="S2" t="n">
+        <v>11.73</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -631,22 +639,22 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>2.94</v>
+        <v>2.98</v>
       </c>
       <c r="L3" t="n">
-        <v>2.94</v>
+        <v>2.98</v>
       </c>
       <c r="M3" t="n">
-        <v>14.84</v>
+        <v>14.79</v>
       </c>
       <c r="N3" t="n">
-        <v>8.75</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="O3" t="n">
-        <v>-21.69</v>
+        <v>-21.46</v>
       </c>
       <c r="P3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q3" t="n">
         <v>4.5</v>
@@ -654,6 +662,9 @@
       <c r="R3" t="n">
         <v>450</v>
       </c>
+      <c r="S3" t="n">
+        <v>5.16</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -699,19 +710,19 @@
         <v>7.06</v>
       </c>
       <c r="K4" t="n">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
       <c r="L4" t="n">
-        <v>9.52</v>
+        <v>9.5</v>
       </c>
       <c r="M4" t="n">
-        <v>8.73</v>
+        <v>8.75</v>
       </c>
       <c r="N4" t="n">
-        <v>5.29</v>
+        <v>5.33</v>
       </c>
       <c r="O4" t="n">
-        <v>-5.18</v>
+        <v>-4.71</v>
       </c>
       <c r="P4" t="n">
         <v>0.86</v>
@@ -722,6 +733,9 @@
       <c r="R4" t="n">
         <v>2100</v>
       </c>
+      <c r="S4" t="n">
+        <v>78.89</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -763,13 +777,13 @@
         <v>1.61</v>
       </c>
       <c r="K5" t="n">
-        <v>1.44</v>
+        <v>1.52</v>
       </c>
       <c r="L5" t="n">
-        <v>3.3</v>
+        <v>3.38</v>
       </c>
       <c r="M5" t="n">
-        <v>7.66</v>
+        <v>7.76</v>
       </c>
       <c r="N5" t="n">
         <v>5.68</v>
@@ -778,7 +792,7 @@
         <v>-9.220000000000001</v>
       </c>
       <c r="P5" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="Q5" t="n">
         <v>0</v>
@@ -786,6 +800,9 @@
       <c r="R5" t="n">
         <v>0</v>
       </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -831,19 +848,19 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>-9.25</v>
+        <v>-9.08</v>
       </c>
       <c r="L6" t="n">
-        <v>-9.25</v>
+        <v>-9.08</v>
       </c>
       <c r="M6" t="n">
-        <v>44.7</v>
+        <v>44.58</v>
       </c>
       <c r="N6" t="n">
-        <v>25.02</v>
+        <v>24.83</v>
       </c>
       <c r="O6" t="n">
-        <v>-82.92</v>
+        <v>-83.44</v>
       </c>
       <c r="P6" t="n">
         <v>-0.25</v>
@@ -854,6 +871,9 @@
       <c r="R6" t="n">
         <v>0</v>
       </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -899,22 +919,22 @@
         <v>1.24</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.28</v>
+        <v>-0.32</v>
       </c>
       <c r="L7" t="n">
-        <v>2.2</v>
+        <v>2.15</v>
       </c>
       <c r="M7" t="n">
-        <v>6.51</v>
+        <v>6.46</v>
       </c>
       <c r="N7" t="n">
         <v>5.96</v>
       </c>
       <c r="O7" t="n">
-        <v>-8.5</v>
+        <v>-8.48</v>
       </c>
       <c r="P7" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
@@ -922,6 +942,9 @@
       <c r="R7" t="n">
         <v>0</v>
       </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -967,27 +990,30 @@
         <v>0.01</v>
       </c>
       <c r="K8" t="n">
-        <v>1.5</v>
+        <v>1.57</v>
       </c>
       <c r="L8" t="n">
-        <v>1.51</v>
+        <v>1.58</v>
       </c>
       <c r="M8" t="n">
-        <v>5.39</v>
+        <v>5.48</v>
       </c>
       <c r="N8" t="n">
         <v>3.49</v>
       </c>
       <c r="O8" t="n">
-        <v>-7.19</v>
+        <v>-7.27</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
       <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1002,7 +1028,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1101,6 +1127,11 @@
           <t>Portfolio Asset Allocation</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Shares</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1142,28 +1173,31 @@
         <v>4.77</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.52</v>
+        <v>-3.6</v>
       </c>
       <c r="L2" t="n">
-        <v>10.77</v>
+        <v>10.68</v>
       </c>
       <c r="M2" t="n">
-        <v>11.02</v>
+        <v>10.94</v>
       </c>
       <c r="N2" t="n">
         <v>10.88</v>
       </c>
       <c r="O2" t="n">
-        <v>-7.64</v>
+        <v>-7.26</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8</v>
+        <v>0.79</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>15.75</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>1575</v>
+      </c>
+      <c r="S2" t="n">
+        <v>78.28</v>
       </c>
     </row>
     <row r="3">
@@ -1207,31 +1241,34 @@
         <v>4.73</v>
       </c>
       <c r="J3" t="n">
-        <v>3.07</v>
+        <v>3.08</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.25</v>
+        <v>-0.4</v>
       </c>
       <c r="L3" t="n">
-        <v>4.48</v>
+        <v>4.33</v>
       </c>
       <c r="M3" t="n">
-        <v>0.4</v>
+        <v>0.32</v>
       </c>
       <c r="N3" t="n">
-        <v>2.27</v>
+        <v>2.41</v>
       </c>
       <c r="O3" t="n">
-        <v>3.82</v>
+        <v>3.81</v>
       </c>
       <c r="P3" t="n">
-        <v>6.15</v>
+        <v>7.4</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>2.63</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>262.64</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2.66</v>
       </c>
     </row>
     <row r="4">
@@ -1269,37 +1306,40 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0.04</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I4" t="n">
         <v>4.92</v>
       </c>
       <c r="J4" t="n">
-        <v>3.19</v>
+        <v>3.2</v>
       </c>
       <c r="K4" t="n">
-        <v>-1.11</v>
+        <v>-1.26</v>
       </c>
       <c r="L4" t="n">
-        <v>3.89</v>
+        <v>3.74</v>
       </c>
       <c r="M4" t="n">
-        <v>18.18</v>
+        <v>18.11</v>
       </c>
       <c r="N4" t="n">
         <v>13.93</v>
       </c>
       <c r="O4" t="n">
-        <v>-26.47</v>
+        <v>-26.33</v>
       </c>
       <c r="P4" t="n">
         <v>0.1</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>2.63</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>262.64</v>
+      </c>
+      <c r="S4" t="n">
+        <v>3.28</v>
       </c>
     </row>
     <row r="5">
@@ -1358,16 +1398,19 @@
         <v>11.04</v>
       </c>
       <c r="O5" t="n">
-        <v>-16.96</v>
+        <v>-16.85</v>
       </c>
       <c r="P5" t="n">
         <v>0.05</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>700</v>
+      </c>
+      <c r="S5" t="n">
+        <v>10.98</v>
       </c>
     </row>
     <row r="6">
@@ -1414,28 +1457,31 @@
         <v>0.57</v>
       </c>
       <c r="K6" t="n">
-        <v>20.36</v>
+        <v>20.41</v>
       </c>
       <c r="L6" t="n">
-        <v>21.07</v>
+        <v>21.12</v>
       </c>
       <c r="M6" t="n">
-        <v>17.62</v>
+        <v>17.65</v>
       </c>
       <c r="N6" t="n">
         <v>4.47</v>
       </c>
       <c r="O6" t="n">
-        <v>-7.04</v>
+        <v>-8.07</v>
       </c>
       <c r="P6" t="n">
         <v>1.08</v>
       </c>
       <c r="Q6" t="n">
-        <v>12.22</v>
+        <v>12</v>
       </c>
       <c r="R6" t="n">
-        <v>1221.6</v>
+        <v>1200</v>
+      </c>
+      <c r="S6" t="n">
+        <v>35.22</v>
       </c>
     </row>
   </sheetData>
@@ -1449,7 +1495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1548,6 +1594,11 @@
           <t>Portfolio Asset Allocation</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Shares</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1584,37 +1635,40 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.03</v>
+        <v>0.14</v>
       </c>
       <c r="I2" t="n">
         <v>1.48</v>
       </c>
       <c r="J2" t="n">
-        <v>1.33</v>
+        <v>1.48</v>
       </c>
       <c r="K2" t="n">
-        <v>13.51</v>
+        <v>13.64</v>
       </c>
       <c r="L2" t="n">
-        <v>15.02</v>
+        <v>15.14</v>
       </c>
       <c r="M2" t="n">
-        <v>20.03</v>
+        <v>20.11</v>
       </c>
       <c r="N2" t="n">
         <v>9.68</v>
       </c>
       <c r="O2" t="n">
-        <v>-17.75</v>
+        <v>-17.79</v>
       </c>
       <c r="P2" t="n">
         <v>0.65</v>
       </c>
       <c r="Q2" t="n">
-        <v>9.24</v>
+        <v>4.8</v>
       </c>
       <c r="R2" t="n">
-        <v>923.62</v>
+        <v>479.52</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1.1</v>
       </c>
     </row>
     <row r="3">
@@ -1661,28 +1715,31 @@
         <v>2.02</v>
       </c>
       <c r="K3" t="n">
-        <v>8.779999999999999</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="L3" t="n">
-        <v>11.68</v>
+        <v>11.78</v>
       </c>
       <c r="M3" t="n">
-        <v>16.71</v>
+        <v>16.7</v>
       </c>
       <c r="N3" t="n">
         <v>7.17</v>
       </c>
       <c r="O3" t="n">
-        <v>-15.72</v>
+        <v>-16.23</v>
       </c>
       <c r="P3" t="n">
-        <v>0.58</v>
+        <v>0.59</v>
       </c>
       <c r="Q3" t="n">
-        <v>4.04</v>
+        <v>2.1</v>
       </c>
       <c r="R3" t="n">
-        <v>404.26</v>
+        <v>209.88</v>
+      </c>
+      <c r="S3" t="n">
+        <v>6.51</v>
       </c>
     </row>
     <row r="4">
@@ -1729,28 +1786,31 @@
         <v>8.77</v>
       </c>
       <c r="K4" t="n">
-        <v>3.76</v>
+        <v>3.86</v>
       </c>
       <c r="L4" t="n">
-        <v>4.6</v>
+        <v>4.7</v>
       </c>
       <c r="M4" t="n">
-        <v>16.38</v>
+        <v>16.39</v>
       </c>
       <c r="N4" t="n">
         <v>11.05</v>
       </c>
       <c r="O4" t="n">
-        <v>-22.17</v>
+        <v>-21.94</v>
       </c>
       <c r="P4" t="n">
         <v>0.16</v>
       </c>
       <c r="Q4" t="n">
-        <v>5.59</v>
+        <v>2.9</v>
       </c>
       <c r="R4" t="n">
-        <v>558.54</v>
+        <v>289.98</v>
+      </c>
+      <c r="S4" t="n">
+        <v>11.31</v>
       </c>
     </row>
     <row r="5">
@@ -1794,31 +1854,34 @@
         <v>3.03</v>
       </c>
       <c r="J5" t="n">
-        <v>2.39</v>
+        <v>2.45</v>
       </c>
       <c r="K5" t="n">
-        <v>5.77</v>
+        <v>5.75</v>
       </c>
       <c r="L5" t="n">
-        <v>8.83</v>
+        <v>8.81</v>
       </c>
       <c r="M5" t="n">
-        <v>15.6</v>
+        <v>15.59</v>
       </c>
       <c r="N5" t="n">
         <v>9.18</v>
       </c>
       <c r="O5" t="n">
-        <v>-16.75</v>
+        <v>-16.71</v>
       </c>
       <c r="P5" t="n">
         <v>0.44</v>
       </c>
       <c r="Q5" t="n">
-        <v>3.47</v>
+        <v>1.8</v>
       </c>
       <c r="R5" t="n">
-        <v>346.7</v>
+        <v>180</v>
+      </c>
+      <c r="S5" t="n">
+        <v>4.55</v>
       </c>
     </row>
     <row r="6">
@@ -1865,10 +1928,10 @@
         <v>3.6</v>
       </c>
       <c r="K6" t="n">
-        <v>4.36</v>
+        <v>4.55</v>
       </c>
       <c r="L6" t="n">
-        <v>8.68</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="M6" t="n">
         <v>10.6</v>
@@ -1877,16 +1940,19 @@
         <v>6</v>
       </c>
       <c r="O6" t="n">
-        <v>-8.359999999999999</v>
+        <v>-8.76</v>
       </c>
       <c r="P6" t="n">
-        <v>0.63</v>
+        <v>0.65</v>
       </c>
       <c r="Q6" t="n">
-        <v>4.82</v>
+        <v>2.5</v>
       </c>
       <c r="R6" t="n">
-        <v>481.57</v>
+        <v>250.02</v>
+      </c>
+      <c r="S6" t="n">
+        <v>9.07</v>
       </c>
     </row>
     <row r="7">
@@ -1930,31 +1996,34 @@
         <v>2.36</v>
       </c>
       <c r="J7" t="n">
-        <v>2.29</v>
+        <v>2.54</v>
       </c>
       <c r="K7" t="n">
-        <v>6.6</v>
+        <v>6.22</v>
       </c>
       <c r="L7" t="n">
-        <v>8.98</v>
+        <v>8.6</v>
       </c>
       <c r="M7" t="n">
-        <v>13.97</v>
+        <v>13.72</v>
       </c>
       <c r="N7" t="n">
         <v>8.69</v>
       </c>
       <c r="O7" t="n">
-        <v>-14.01</v>
+        <v>-14.03</v>
       </c>
       <c r="P7" t="n">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="Q7" t="n">
-        <v>7.53</v>
+        <v>3.91</v>
       </c>
       <c r="R7" t="n">
-        <v>752.6900000000001</v>
+        <v>390.78</v>
+      </c>
+      <c r="S7" t="n">
+        <v>7.05</v>
       </c>
     </row>
     <row r="8">
@@ -1998,31 +2067,34 @@
         <v>12.91</v>
       </c>
       <c r="J8" t="n">
-        <v>13.26</v>
+        <v>11.74</v>
       </c>
       <c r="K8" t="n">
-        <v>-1.55</v>
+        <v>-2.23</v>
       </c>
       <c r="L8" t="n">
-        <v>11.39</v>
+        <v>10.71</v>
       </c>
       <c r="M8" t="n">
-        <v>8.18</v>
+        <v>8.710000000000001</v>
       </c>
       <c r="N8" t="n">
-        <v>7.08</v>
+        <v>7.87</v>
       </c>
       <c r="O8" t="n">
-        <v>-1.79</v>
+        <v>-3.2</v>
       </c>
       <c r="P8" t="n">
-        <v>1.15</v>
+        <v>1</v>
       </c>
       <c r="Q8" t="n">
-        <v>23.11</v>
+        <v>12</v>
       </c>
       <c r="R8" t="n">
-        <v>2311.36</v>
+        <v>1200</v>
+      </c>
+      <c r="S8" t="n">
+        <v>89.15000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -2062,30 +2134,33 @@
         <v>0.64</v>
       </c>
       <c r="J9" t="n">
-        <v>1.29</v>
+        <v>2.08</v>
       </c>
       <c r="K9" t="n">
-        <v>11.91</v>
+        <v>11.17</v>
       </c>
       <c r="L9" t="n">
-        <v>12.57</v>
+        <v>11.82</v>
       </c>
       <c r="M9" t="n">
-        <v>30.85</v>
+        <v>31.33</v>
       </c>
       <c r="N9" t="n">
-        <v>10.44</v>
+        <v>10.79</v>
       </c>
       <c r="O9" t="n">
-        <v>-37.5</v>
+        <v>-38.94</v>
       </c>
       <c r="P9" t="n">
-        <v>0.34</v>
+        <v>0.31</v>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
       <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>